<commit_message>
Reviewed page access logic
</commit_message>
<xml_diff>
--- a/tools/web file descriptions.xlsx
+++ b/tools/web file descriptions.xlsx
@@ -14,14 +14,14 @@
     <sheet name="Sheet3" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Current!$A$1:$O$138</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Current!$A$1:$O$139</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1258" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1272" uniqueCount="389">
   <si>
     <t>addPatient.php</t>
   </si>
@@ -1219,6 +1219,15 @@
   </si>
   <si>
     <t>pass</t>
+  </si>
+  <si>
+    <t>uihelp</t>
+  </si>
+  <si>
+    <t>favicon.ico</t>
+  </si>
+  <si>
+    <t>FavIcon file</t>
   </si>
 </sst>
 </file>
@@ -1575,20 +1584,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O138"/>
+  <dimension ref="A1:O139"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="555" activePane="bottomLeft"/>
-      <selection activeCell="D1" sqref="D1:D1048576"/>
-      <selection pane="bottomLeft" activeCell="A81" sqref="A81"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="4"/>
     <col min="2" max="2" width="29" customWidth="1"/>
-    <col min="3" max="5" width="10" customWidth="1"/>
-    <col min="6" max="7" width="43.85546875" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="4" max="5" width="10" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="43.85546875" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="44.42578125" customWidth="1"/>
     <col min="8" max="13" width="20.7109375" customWidth="1"/>
     <col min="14" max="14" width="36" customWidth="1"/>
     <col min="15" max="15" width="48" customWidth="1"/>
@@ -1652,7 +1659,7 @@
         <v>294</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="H2"/>
       <c r="I2"/>
@@ -1664,7 +1671,9 @@
       <c r="O2"/>
     </row>
     <row r="3" spans="1:15" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
+      <c r="A3" s="4" t="s">
+        <v>386</v>
+      </c>
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1692,7 +1701,9 @@
       </c>
     </row>
     <row r="4" spans="1:15" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
+      <c r="A4" s="4" t="s">
+        <v>384</v>
+      </c>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
@@ -1754,7 +1765,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>355</v>
+        <v>386</v>
       </c>
       <c r="B6" t="s">
         <v>243</v>
@@ -2025,6 +2036,9 @@
       </c>
       <c r="C17" t="s">
         <v>31</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>222</v>
       </c>
       <c r="I17" s="1"/>
     </row>
@@ -2287,6 +2301,9 @@
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>359</v>
+      </c>
       <c r="B28" s="1" t="s">
         <v>190</v>
       </c>
@@ -2500,6 +2517,9 @@
       <c r="O35"/>
     </row>
     <row r="36" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>384</v>
+      </c>
       <c r="B36" s="1" t="s">
         <v>119</v>
       </c>
@@ -2534,7 +2554,7 @@
     </row>
     <row r="37" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>355</v>
+        <v>386</v>
       </c>
       <c r="B37" t="s">
         <v>191</v>
@@ -2549,7 +2569,7 @@
         <v>204</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I37" s="1" t="str">
         <f>VLOOKUP(B37,Profiled!A$1:A$98,1,FALSE)</f>
@@ -2564,20 +2584,18 @@
     </row>
     <row r="38" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>363</v>
-      </c>
-      <c r="B38" t="s">
-        <v>275</v>
-      </c>
-      <c r="C38" t="s">
-        <v>223</v>
+        <v>355</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="D38"/>
-      <c r="E38" t="s">
-        <v>242</v>
-      </c>
-      <c r="F38" t="s">
-        <v>279</v>
+      <c r="E38"/>
+      <c r="F38" s="1" t="s">
+        <v>388</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>222</v>
@@ -2593,44 +2611,42 @@
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>355</v>
+        <v>363</v>
       </c>
       <c r="B39" t="s">
-        <v>290</v>
+        <v>275</v>
       </c>
       <c r="C39" t="s">
-        <v>31</v>
-      </c>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1" t="s">
-        <v>240</v>
+        <v>223</v>
+      </c>
+      <c r="E39" t="s">
+        <v>242</v>
       </c>
       <c r="F39" t="s">
-        <v>301</v>
+        <v>279</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
     </row>
     <row r="40" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="B40" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C40" t="s">
-        <v>67</v>
-      </c>
-      <c r="D40"/>
-      <c r="E40" t="s">
-        <v>242</v>
+        <v>31</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>240</v>
       </c>
       <c r="F40" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="H40"/>
       <c r="I40"/>
@@ -2643,22 +2659,22 @@
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>370</v>
+        <v>359</v>
       </c>
       <c r="B41" t="s">
-        <v>319</v>
+        <v>291</v>
       </c>
       <c r="C41" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
       <c r="E41" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="F41" t="s">
-        <v>327</v>
+        <v>302</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
     </row>
     <row r="42" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2666,17 +2682,17 @@
         <v>370</v>
       </c>
       <c r="B42" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C42" t="s">
         <v>29</v>
       </c>
       <c r="D42"/>
       <c r="E42" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F42" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>219</v>
@@ -2695,7 +2711,7 @@
         <v>370</v>
       </c>
       <c r="B43" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C43" t="s">
         <v>29</v>
@@ -2705,7 +2721,7 @@
         <v>242</v>
       </c>
       <c r="F43" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>219</v>
@@ -2724,7 +2740,7 @@
         <v>370</v>
       </c>
       <c r="B44" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C44" t="s">
         <v>29</v>
@@ -2734,10 +2750,10 @@
         <v>242</v>
       </c>
       <c r="F44" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="H44"/>
       <c r="I44"/>
@@ -2750,23 +2766,23 @@
     </row>
     <row r="45" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B45" t="s">
-        <v>368</v>
+        <v>322</v>
       </c>
       <c r="C45" t="s">
-        <v>325</v>
+        <v>29</v>
       </c>
       <c r="D45"/>
-      <c r="E45" s="1" t="s">
-        <v>239</v>
+      <c r="E45" t="s">
+        <v>242</v>
       </c>
       <c r="F45" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H45"/>
       <c r="I45"/>
@@ -2779,36 +2795,31 @@
     </row>
     <row r="46" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>384</v>
+        <v>369</v>
       </c>
       <c r="B46" t="s">
-        <v>7</v>
+        <v>368</v>
       </c>
       <c r="C46" t="s">
-        <v>29</v>
+        <v>325</v>
       </c>
       <c r="D46"/>
-      <c r="E46" t="s">
-        <v>241</v>
+      <c r="E46" s="1" t="s">
+        <v>239</v>
       </c>
       <c r="F46" t="s">
-        <v>41</v>
+        <v>326</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>222</v>
       </c>
       <c r="H46"/>
-      <c r="I46" s="1" t="str">
-        <f>VLOOKUP(B46,Profiled!A$1:A$98,1,FALSE)</f>
-        <v>image.php</v>
-      </c>
+      <c r="I46"/>
       <c r="J46"/>
       <c r="K46"/>
       <c r="L46"/>
       <c r="M46"/>
-      <c r="N46" t="s">
-        <v>183</v>
-      </c>
+      <c r="N46"/>
       <c r="O46"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
@@ -2816,22 +2827,23 @@
         <v>384</v>
       </c>
       <c r="B47" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C47" t="s">
         <v>29</v>
       </c>
       <c r="E47" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F47" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="I47" s="1" t="s">
-        <v>271</v>
+      <c r="I47" s="1" t="str">
+        <f>VLOOKUP(B47,Profiled!A$1:A$98,1,FALSE)</f>
+        <v>image.php</v>
       </c>
       <c r="N47" t="s">
         <v>183</v>
@@ -2842,7 +2854,7 @@
         <v>384</v>
       </c>
       <c r="B48" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C48" t="s">
         <v>29</v>
@@ -2851,17 +2863,16 @@
         <v>242</v>
       </c>
       <c r="F48" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="I48" s="1" t="str">
-        <f>VLOOKUP(B48,Profiled!A$1:A$98,1,FALSE)</f>
-        <v>image_delete.php</v>
+        <v>222</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>271</v>
       </c>
       <c r="N48" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
@@ -2869,7 +2880,7 @@
         <v>384</v>
       </c>
       <c r="B49" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C49" t="s">
         <v>29</v>
@@ -2878,14 +2889,14 @@
         <v>242</v>
       </c>
       <c r="F49" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="I49" s="1" t="str">
         <f>VLOOKUP(B49,Profiled!A$1:A$98,1,FALSE)</f>
-        <v>image_get.php</v>
+        <v>image_delete.php</v>
       </c>
       <c r="N49" t="s">
         <v>188</v>
@@ -2896,7 +2907,7 @@
         <v>384</v>
       </c>
       <c r="B50" t="s">
-        <v>120</v>
+        <v>10</v>
       </c>
       <c r="C50" t="s">
         <v>29</v>
@@ -2906,15 +2917,15 @@
         <v>242</v>
       </c>
       <c r="F50" t="s">
-        <v>124</v>
+        <v>44</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="H50"/>
       <c r="I50" s="1" t="str">
         <f>VLOOKUP(B50,Profiled!A$1:A$98,1,FALSE)</f>
-        <v>image_patch.php</v>
+        <v>image_get.php</v>
       </c>
       <c r="J50"/>
       <c r="K50"/>
@@ -2930,7 +2941,7 @@
         <v>384</v>
       </c>
       <c r="B51" t="s">
-        <v>11</v>
+        <v>120</v>
       </c>
       <c r="C51" t="s">
         <v>29</v>
@@ -2939,14 +2950,14 @@
         <v>242</v>
       </c>
       <c r="F51" t="s">
-        <v>45</v>
+        <v>124</v>
       </c>
       <c r="G51" s="1" t="s">
         <v>221</v>
       </c>
       <c r="I51" s="1" t="str">
         <f>VLOOKUP(B51,Profiled!A$1:A$98,1,FALSE)</f>
-        <v>image_post.php</v>
+        <v>image_patch.php</v>
       </c>
       <c r="N51" t="s">
         <v>188</v>
@@ -2957,7 +2968,7 @@
         <v>384</v>
       </c>
       <c r="B52" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C52" t="s">
         <v>29</v>
@@ -2967,7 +2978,7 @@
         <v>242</v>
       </c>
       <c r="F52" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>221</v>
@@ -2975,7 +2986,7 @@
       <c r="H52"/>
       <c r="I52" s="1" t="str">
         <f>VLOOKUP(B52,Profiled!A$1:A$98,1,FALSE)</f>
-        <v>image_put.php</v>
+        <v>image_post.php</v>
       </c>
       <c r="J52"/>
       <c r="K52"/>
@@ -2988,35 +2999,51 @@
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>355</v>
+        <v>384</v>
       </c>
       <c r="B53" t="s">
-        <v>357</v>
+        <v>12</v>
       </c>
       <c r="C53" t="s">
-        <v>31</v>
-      </c>
-      <c r="G53" s="1"/>
+        <v>29</v>
+      </c>
+      <c r="E53" t="s">
+        <v>242</v>
+      </c>
+      <c r="F53" t="s">
+        <v>46</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="I53" s="1" t="str">
+        <f>VLOOKUP(B53,Profiled!A$1:A$98,1,FALSE)</f>
+        <v>image_put.php</v>
+      </c>
+      <c r="N53" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>370</v>
+        <v>355</v>
       </c>
       <c r="B54" t="s">
-        <v>374</v>
+        <v>357</v>
       </c>
       <c r="C54" t="s">
-        <v>29</v>
-      </c>
-      <c r="G54" s="1"/>
-      <c r="I54" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>370</v>
       </c>
       <c r="B55" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C55" t="s">
         <v>29</v>
@@ -3029,7 +3056,7 @@
         <v>370</v>
       </c>
       <c r="B56" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C56" t="s">
         <v>29</v>
@@ -3042,7 +3069,7 @@
         <v>370</v>
       </c>
       <c r="B57" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C57" t="s">
         <v>29</v>
@@ -3052,95 +3079,82 @@
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>363</v>
+        <v>370</v>
       </c>
       <c r="B58" t="s">
-        <v>364</v>
+        <v>377</v>
       </c>
       <c r="C58" t="s">
-        <v>97</v>
+        <v>29</v>
       </c>
       <c r="G58" s="1"/>
+      <c r="I58" s="1"/>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>384</v>
+        <v>363</v>
       </c>
       <c r="B59" t="s">
-        <v>192</v>
-      </c>
-      <c r="C59" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="C59" t="s">
         <v>97</v>
       </c>
-      <c r="D59" s="1"/>
-      <c r="E59" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="G59" t="s">
-        <v>222</v>
-      </c>
-      <c r="H59" s="1"/>
-      <c r="I59" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="J59" s="1"/>
-      <c r="K59" s="1"/>
-      <c r="L59" s="1"/>
-      <c r="M59" s="1"/>
-      <c r="N59" s="1"/>
-      <c r="O59" s="1"/>
+      <c r="G59" s="1"/>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>370</v>
+        <v>384</v>
       </c>
       <c r="B60" t="s">
-        <v>13</v>
-      </c>
-      <c r="C60" t="s">
-        <v>29</v>
-      </c>
-      <c r="E60" t="s">
-        <v>241</v>
-      </c>
-      <c r="F60" t="s">
-        <v>49</v>
-      </c>
-      <c r="G60" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G60" t="s">
         <v>222</v>
       </c>
-      <c r="I60" s="1" t="str">
-        <f>VLOOKUP(B60,Profiled!A$1:A$98,1,FALSE)</f>
-        <v>patient.php</v>
-      </c>
-      <c r="N60" t="s">
-        <v>184</v>
-      </c>
+      <c r="H60" s="1"/>
+      <c r="I60" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="J60" s="1"/>
+      <c r="K60" s="1"/>
+      <c r="L60" s="1"/>
+      <c r="M60" s="1"/>
+      <c r="N60" s="1"/>
+      <c r="O60" s="1"/>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>370</v>
       </c>
       <c r="B61" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C61" t="s">
         <v>29</v>
       </c>
       <c r="E61" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F61" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="G61" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="I61" s="1" t="s">
-        <v>271</v>
+      <c r="I61" s="1" t="str">
+        <f>VLOOKUP(B61,Profiled!A$1:A$98,1,FALSE)</f>
+        <v>patient.php</v>
       </c>
       <c r="N61" t="s">
         <v>184</v>
@@ -3151,7 +3165,7 @@
         <v>370</v>
       </c>
       <c r="B62" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C62" t="s">
         <v>29</v>
@@ -3161,22 +3175,21 @@
         <v>242</v>
       </c>
       <c r="F62" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H62"/>
-      <c r="I62" s="1" t="str">
-        <f>VLOOKUP(B62,Profiled!A$1:A$98,1,FALSE)</f>
-        <v>patient_delete.php</v>
+      <c r="I62" s="1" t="s">
+        <v>271</v>
       </c>
       <c r="J62"/>
       <c r="K62"/>
       <c r="L62"/>
       <c r="M62"/>
       <c r="N62" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="O62"/>
     </row>
@@ -3185,7 +3198,7 @@
         <v>370</v>
       </c>
       <c r="B63" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C63" t="s">
         <v>29</v>
@@ -3194,14 +3207,14 @@
         <v>242</v>
       </c>
       <c r="F63" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="I63" s="1" t="str">
         <f>VLOOKUP(B63,Profiled!A$1:A$98,1,FALSE)</f>
-        <v>patient_get.php</v>
+        <v>patient_delete.php</v>
       </c>
       <c r="N63" t="s">
         <v>188</v>
@@ -3212,7 +3225,7 @@
         <v>370</v>
       </c>
       <c r="B64" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C64" t="s">
         <v>29</v>
@@ -3222,15 +3235,15 @@
         <v>242</v>
       </c>
       <c r="F64" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H64"/>
       <c r="I64" s="1" t="str">
         <f>VLOOKUP(B64,Profiled!A$1:A$98,1,FALSE)</f>
-        <v>patient_patch.php</v>
+        <v>patient_get.php</v>
       </c>
       <c r="J64"/>
       <c r="K64"/>
@@ -3246,7 +3259,7 @@
         <v>370</v>
       </c>
       <c r="B65" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C65" t="s">
         <v>29</v>
@@ -3255,14 +3268,14 @@
         <v>242</v>
       </c>
       <c r="F65" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G65" s="1" t="s">
         <v>221</v>
       </c>
       <c r="I65" s="1" t="str">
         <f>VLOOKUP(B65,Profiled!A$1:A$98,1,FALSE)</f>
-        <v>patient_post.php</v>
+        <v>patient_patch.php</v>
       </c>
       <c r="N65" t="s">
         <v>188</v>
@@ -3270,81 +3283,82 @@
     </row>
     <row r="66" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>355</v>
+        <v>370</v>
       </c>
       <c r="B66" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C66" t="s">
-        <v>97</v>
+        <v>29</v>
       </c>
       <c r="D66"/>
       <c r="E66" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="F66" t="s">
-        <v>105</v>
-      </c>
-      <c r="G66" t="s">
-        <v>222</v>
-      </c>
-      <c r="H66" t="s">
-        <v>106</v>
-      </c>
-      <c r="I66" s="1" t="s">
-        <v>271</v>
+        <v>53</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="H66"/>
+      <c r="I66" s="1" t="str">
+        <f>VLOOKUP(B66,Profiled!A$1:A$98,1,FALSE)</f>
+        <v>patient_post.php</v>
       </c>
       <c r="J66"/>
       <c r="K66"/>
       <c r="L66"/>
       <c r="M66"/>
-      <c r="N66"/>
+      <c r="N66" t="s">
+        <v>188</v>
+      </c>
       <c r="O66"/>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>366</v>
+        <v>355</v>
       </c>
       <c r="B67" t="s">
-        <v>367</v>
+        <v>19</v>
       </c>
       <c r="C67" t="s">
-        <v>305</v>
-      </c>
-      <c r="E67" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E67" t="s">
         <v>239</v>
       </c>
       <c r="F67" t="s">
-        <v>306</v>
-      </c>
-      <c r="G67" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G67" t="s">
         <v>222</v>
+      </c>
+      <c r="H67" t="s">
+        <v>106</v>
+      </c>
+      <c r="I67" s="1" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="B68" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="C68" t="s">
-        <v>97</v>
-      </c>
-      <c r="E68" t="s">
-        <v>242</v>
+        <v>305</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>239</v>
       </c>
       <c r="F68" t="s">
-        <v>35</v>
-      </c>
-      <c r="G68" t="s">
+        <v>306</v>
+      </c>
+      <c r="G68" s="1" t="s">
         <v>222</v>
-      </c>
-      <c r="I68" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="N68" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.25">
@@ -3352,147 +3366,141 @@
         <v>363</v>
       </c>
       <c r="B69" t="s">
-        <v>268</v>
-      </c>
-      <c r="C69" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="C69" t="s">
         <v>97</v>
       </c>
-      <c r="D69" s="1"/>
       <c r="E69" t="s">
         <v>242</v>
       </c>
-      <c r="F69" s="1" t="s">
-        <v>269</v>
+      <c r="F69" t="s">
+        <v>35</v>
       </c>
       <c r="G69" t="s">
         <v>222</v>
       </c>
-      <c r="I69" s="1" t="str">
-        <f>VLOOKUP(B69,Profiled!A$1:A$98,1,FALSE)</f>
+      <c r="I69" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="N69" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="B70" t="s">
+        <v>268</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E70" t="s">
+        <v>242</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="G70" t="s">
+        <v>222</v>
+      </c>
+      <c r="H70"/>
+      <c r="I70" s="1" t="str">
+        <f>VLOOKUP(B70,Profiled!A$1:A$98,1,FALSE)</f>
         <v>profile.php</v>
       </c>
-    </row>
-    <row r="70" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="4"/>
-      <c r="B70" s="1" t="s">
+      <c r="J70"/>
+      <c r="K70"/>
+      <c r="L70"/>
+      <c r="M70"/>
+      <c r="N70"/>
+      <c r="O70"/>
+    </row>
+    <row r="71" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="B71" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C70" s="1" t="s">
+      <c r="C71" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E70" s="1" t="s">
+      <c r="E71" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="F70" s="1" t="s">
+      <c r="F71" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G70" s="1" t="s">
+      <c r="G71" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="H70" s="1" t="s">
+      <c r="H71" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="I70" s="1" t="e">
-        <f>VLOOKUP(B70,Profiled!A$1:A$98,1,FALSE)</f>
+      <c r="I71" s="1" t="e">
+        <f>VLOOKUP(B71,Profiled!A$1:A$98,1,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="K70" s="1" t="s">
+      <c r="K71" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="L70" s="1" t="s">
+      <c r="L71" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="M70" s="1" t="s">
+      <c r="M71" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="N70" s="1" t="s">
+      <c r="N71" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="O70" s="1" t="s">
+      <c r="O71" s="1" t="s">
         <v>131</v>
-      </c>
-    </row>
-    <row r="71" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="4"/>
-      <c r="B71" t="s">
-        <v>70</v>
-      </c>
-      <c r="C71" t="s">
-        <v>67</v>
-      </c>
-      <c r="D71"/>
-      <c r="E71" t="s">
-        <v>242</v>
-      </c>
-      <c r="F71" t="s">
-        <v>79</v>
-      </c>
-      <c r="G71" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="H71"/>
-      <c r="I71" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="J71"/>
-      <c r="K71"/>
-      <c r="L71"/>
-      <c r="M71"/>
-      <c r="N71" t="s">
-        <v>158</v>
-      </c>
-      <c r="O71" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="72" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
-        <v>384</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="F72" s="1" t="s">
-        <v>125</v>
+        <v>359</v>
+      </c>
+      <c r="B72" t="s">
+        <v>70</v>
+      </c>
+      <c r="C72" t="s">
+        <v>67</v>
+      </c>
+      <c r="D72"/>
+      <c r="E72" t="s">
+        <v>242</v>
+      </c>
+      <c r="F72" t="s">
+        <v>79</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="H72" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="I72" s="1" t="e">
-        <f>VLOOKUP(B72,Profiled!A$1:A$98,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="K72" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="L72" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="M72" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="N72" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="O72" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="73" spans="1:15" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+        <v>222</v>
+      </c>
+      <c r="H72"/>
+      <c r="I72" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="J72"/>
+      <c r="K72"/>
+      <c r="L72"/>
+      <c r="M72"/>
+      <c r="N72" t="s">
+        <v>158</v>
+      </c>
+      <c r="O72" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>384</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>88</v>
+        <v>121</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>31</v>
@@ -3501,7 +3509,7 @@
         <v>240</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>38</v>
+        <v>125</v>
       </c>
       <c r="G73" s="1" t="s">
         <v>221</v>
@@ -3522,315 +3530,320 @@
       <c r="M73" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="N73" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="O73" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="74" spans="1:15" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="N73" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="O73" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>384</v>
       </c>
       <c r="B74" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="H74" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="I74" s="1" t="e">
+        <f>VLOOKUP(B74,Profiled!A$1:A$98,1,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K74" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="L74" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="M74" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="N74" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="O74" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A75" s="4" t="s">
+        <v>384</v>
+      </c>
+      <c r="B75" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C74" s="1" t="s">
+      <c r="C75" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E74" s="1" t="s">
+      <c r="E75" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="F74" s="1" t="s">
+      <c r="F75" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="G74" s="1" t="s">
+      <c r="G75" s="1" t="s">
         <v>222</v>
-      </c>
-      <c r="I74" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="N74" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="O74" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="75" spans="1:15" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A75" s="4" t="s">
-        <v>355</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="F75" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G75" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="H75" s="1" t="s">
-        <v>217</v>
       </c>
       <c r="I75" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="K75" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="L75" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="M75" s="1" t="s">
-        <v>230</v>
-      </c>
       <c r="N75" s="2" t="s">
-        <v>136</v>
+        <v>166</v>
       </c>
       <c r="O75" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="76" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
-        <v>359</v>
-      </c>
-      <c r="B76" t="s">
-        <v>72</v>
-      </c>
-      <c r="C76" t="s">
-        <v>67</v>
-      </c>
-      <c r="D76"/>
-      <c r="E76" t="s">
-        <v>242</v>
-      </c>
-      <c r="F76" t="s">
-        <v>81</v>
+        <v>355</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="H76"/>
+        <v>220</v>
+      </c>
+      <c r="H76" s="1" t="s">
+        <v>217</v>
+      </c>
       <c r="I76" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="J76"/>
-      <c r="K76"/>
-      <c r="L76"/>
-      <c r="M76"/>
-      <c r="N76" t="s">
-        <v>159</v>
-      </c>
-      <c r="O76" t="s">
-        <v>157</v>
+      <c r="K76" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="L76" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="M76" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="N76" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="O76" s="2" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="77" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
-        <v>355</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="F77" s="1" t="s">
-        <v>55</v>
+        <v>359</v>
+      </c>
+      <c r="B77" t="s">
+        <v>72</v>
+      </c>
+      <c r="C77" t="s">
+        <v>67</v>
+      </c>
+      <c r="D77"/>
+      <c r="E77" t="s">
+        <v>242</v>
+      </c>
+      <c r="F77" t="s">
+        <v>81</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="H77" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="I77" s="1" t="e">
-        <f>VLOOKUP(B77,Profiled!A$1:A$98,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="K77" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="L77" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="M77" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="N77" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="O77" s="1" t="s">
-        <v>139</v>
+        <v>222</v>
+      </c>
+      <c r="H77"/>
+      <c r="I77" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="J77"/>
+      <c r="K77"/>
+      <c r="L77"/>
+      <c r="M77"/>
+      <c r="N77" t="s">
+        <v>159</v>
+      </c>
+      <c r="O77" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="78" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
-        <v>359</v>
-      </c>
-      <c r="B78" t="s">
-        <v>73</v>
-      </c>
-      <c r="C78" t="s">
-        <v>67</v>
-      </c>
-      <c r="D78"/>
-      <c r="E78" t="s">
-        <v>242</v>
-      </c>
-      <c r="F78" t="s">
-        <v>82</v>
+        <v>355</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="H78"/>
-      <c r="I78" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="J78"/>
-      <c r="K78"/>
-      <c r="L78"/>
-      <c r="M78"/>
-      <c r="N78" t="s">
-        <v>160</v>
-      </c>
-      <c r="O78" t="s">
-        <v>157</v>
+        <v>219</v>
+      </c>
+      <c r="H78" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="I78" s="1" t="e">
+        <f>VLOOKUP(B78,Profiled!A$1:A$98,1,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K78" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="L78" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="M78" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="N78" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="O78" s="1" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="79" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
-        <v>384</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="F79" s="1" t="s">
-        <v>40</v>
+        <v>359</v>
+      </c>
+      <c r="B79" t="s">
+        <v>73</v>
+      </c>
+      <c r="C79" t="s">
+        <v>67</v>
+      </c>
+      <c r="D79"/>
+      <c r="E79" t="s">
+        <v>242</v>
+      </c>
+      <c r="F79" t="s">
+        <v>82</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="H79" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="I79" s="1" t="e">
-        <f>VLOOKUP(B79,Profiled!A$1:A$98,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="K79" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="L79" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="M79" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="N79" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="O79" s="1" t="s">
-        <v>139</v>
+        <v>222</v>
+      </c>
+      <c r="H79"/>
+      <c r="I79" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="J79"/>
+      <c r="K79"/>
+      <c r="L79"/>
+      <c r="M79"/>
+      <c r="N79" t="s">
+        <v>160</v>
+      </c>
+      <c r="O79" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="80" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>384</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B80" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="H80" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="I80" s="1" t="e">
+        <f>VLOOKUP(B80,Profiled!A$1:A$98,1,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K80" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="L80" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="M80" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="N80" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="O80" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="4" t="s">
+        <v>384</v>
+      </c>
+      <c r="B81" t="s">
         <v>74</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C81" t="s">
         <v>67</v>
       </c>
-      <c r="D80"/>
-      <c r="E80" t="s">
+      <c r="D81"/>
+      <c r="E81" t="s">
         <v>242</v>
       </c>
-      <c r="F80" t="s">
+      <c r="F81" t="s">
         <v>83</v>
       </c>
-      <c r="G80" s="1" t="s">
+      <c r="G81" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="H80"/>
-      <c r="I80" s="1" t="s">
+      <c r="H81"/>
+      <c r="I81" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="J80"/>
-      <c r="K80"/>
-      <c r="L80"/>
-      <c r="M80"/>
-      <c r="N80" t="s">
+      <c r="J81"/>
+      <c r="K81"/>
+      <c r="L81"/>
+      <c r="M81"/>
+      <c r="N81" t="s">
         <v>161</v>
       </c>
-      <c r="O80" t="s">
+      <c r="O81" t="s">
         <v>157</v>
-      </c>
-    </row>
-    <row r="81" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="4"/>
-      <c r="B81" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E81" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="F81" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="G81" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="H81" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="I81" s="1" t="e">
-        <f>VLOOKUP(B81,Profiled!A$1:A$98,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="K81" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="L81" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="N81" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="O81" s="1" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="82" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
-        <v>355</v>
+        <v>384</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>358</v>
+        <v>122</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>31</v>
@@ -3839,10 +3852,10 @@
         <v>240</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="H82" s="1" t="s">
         <v>217</v>
@@ -3857,331 +3870,337 @@
       <c r="L82" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="M82" s="1" t="s">
-        <v>229</v>
-      </c>
       <c r="N82" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="O82" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="83" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="H83" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="I83" s="1" t="e">
+        <f>VLOOKUP(B83,Profiled!A$1:A$98,1,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K83" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="L83" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="M83" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="N83" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="O83" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="4" t="s">
         <v>359</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="B84" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="C83" s="1" t="s">
+      <c r="C84" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E83" t="s">
+      <c r="E84" t="s">
         <v>242</v>
       </c>
-      <c r="F83" s="1" t="s">
+      <c r="F84" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="G83" s="1" t="s">
+      <c r="G84" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="I83" s="1" t="s">
+      <c r="I84" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="N83" s="1" t="s">
+      <c r="N84" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="O83" t="s">
+      <c r="O84" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="84" spans="1:15" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A84" s="4"/>
-      <c r="B84" s="1" t="s">
+    <row r="85" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="B85" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C84" s="1" t="s">
+      <c r="C85" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E84" s="1" t="s">
+      <c r="D85" s="1"/>
+      <c r="E85" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="F84" s="1" t="s">
+      <c r="F85" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="G84" s="1" t="s">
+      <c r="G85" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="H84" s="1" t="s">
+      <c r="H85" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="I84" s="1" t="e">
-        <f>VLOOKUP(B84,Profiled!A$1:A$98,1,FALSE)</f>
+      <c r="I85" s="1" t="e">
+        <f>VLOOKUP(B85,Profiled!A$1:A$98,1,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="K84" s="1" t="s">
+      <c r="J85" s="1"/>
+      <c r="K85" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="L84" s="1" t="s">
+      <c r="L85" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="M84" s="1" t="s">
+      <c r="M85" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="N84" s="2" t="s">
+      <c r="N85" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="O84" s="2" t="s">
+      <c r="O85" s="2" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B85" s="1" t="s">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B86" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C85" s="1" t="s">
+      <c r="C86" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D85" s="1"/>
-      <c r="E85" t="s">
+      <c r="D86" s="1"/>
+      <c r="E86" t="s">
         <v>242</v>
       </c>
-      <c r="F85" s="1" t="s">
+      <c r="F86" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="G85" s="1" t="s">
+      <c r="G86" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="H85" s="1"/>
-      <c r="I85" s="1" t="s">
+      <c r="H86" s="1"/>
+      <c r="I86" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="J85" s="1"/>
-      <c r="K85" s="1"/>
-      <c r="L85" s="1"/>
-      <c r="M85" s="1"/>
-      <c r="N85" s="1" t="s">
+      <c r="J86" s="1"/>
+      <c r="K86" s="1"/>
+      <c r="L86" s="1"/>
+      <c r="M86" s="1"/>
+      <c r="N86" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="O85" t="s">
+      <c r="O86" t="s">
         <v>157</v>
-      </c>
-    </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B86" t="s">
-        <v>347</v>
-      </c>
-      <c r="C86" t="s">
-        <v>31</v>
-      </c>
-      <c r="D86" s="1"/>
-      <c r="E86" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="F86" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="G86" s="1" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C87" t="s">
-        <v>67</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="D87" s="1"/>
       <c r="E87" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="88" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C88" t="s">
-        <v>31</v>
-      </c>
-      <c r="D88" s="1"/>
+        <v>67</v>
+      </c>
       <c r="E88" s="1" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>308</v>
+        <v>349</v>
       </c>
       <c r="C89" t="s">
         <v>31</v>
       </c>
       <c r="D89" s="1"/>
-      <c r="E89" t="s">
+      <c r="E89" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="F89" t="s">
-        <v>311</v>
+      <c r="F89" s="1" t="s">
+        <v>353</v>
       </c>
       <c r="G89" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="N89" t="s">
-        <v>316</v>
-      </c>
-      <c r="O89" t="s">
-        <v>317</v>
-      </c>
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>343</v>
+        <v>308</v>
       </c>
       <c r="C90" t="s">
         <v>31</v>
       </c>
       <c r="D90" s="1"/>
-      <c r="E90" s="1" t="s">
+      <c r="E90" t="s">
         <v>240</v>
       </c>
       <c r="F90" t="s">
-        <v>346</v>
-      </c>
-      <c r="G90" t="s">
+        <v>311</v>
+      </c>
+      <c r="G90" s="1" t="s">
         <v>220</v>
+      </c>
+      <c r="N90" t="s">
+        <v>316</v>
+      </c>
+      <c r="O90" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
+        <v>343</v>
+      </c>
+      <c r="C91" t="s">
+        <v>31</v>
+      </c>
+      <c r="D91" s="1"/>
+      <c r="E91" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="F91" t="s">
+        <v>346</v>
+      </c>
+      <c r="G91" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
         <v>309</v>
       </c>
-      <c r="C91" t="s">
+      <c r="C92" t="s">
         <v>67</v>
       </c>
-      <c r="E91" s="1" t="s">
+      <c r="E92" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="F91" t="s">
+      <c r="F92" t="s">
         <v>312</v>
       </c>
-      <c r="G91" s="1" t="s">
+      <c r="G92" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="N91" t="s">
+      <c r="N92" t="s">
         <v>318</v>
       </c>
-      <c r="O91" t="s">
+      <c r="O92" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A92" s="4" t="s">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A93" s="4" t="s">
         <v>363</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B93" t="s">
         <v>193</v>
       </c>
-      <c r="C92" s="1" t="s">
+      <c r="C93" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="D92" s="1"/>
-      <c r="E92" t="s">
-        <v>242</v>
-      </c>
-      <c r="F92" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="G92" t="s">
-        <v>222</v>
-      </c>
-      <c r="H92" s="1"/>
-      <c r="I92" s="1" t="str">
-        <f>VLOOKUP(B92,Profiled!A$1:A$98,1,FALSE)</f>
-        <v>security.php</v>
-      </c>
-      <c r="J92" s="1"/>
-      <c r="K92" s="1"/>
-      <c r="L92" s="1"/>
-      <c r="M92" s="1"/>
-      <c r="N92" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="O92" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B93" t="s">
-        <v>232</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="D93" s="1"/>
       <c r="E93" t="s">
         <v>242</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="G93" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="G93" t="s">
         <v>222</v>
       </c>
       <c r="H93" s="1"/>
-      <c r="I93" s="1" t="s">
-        <v>271</v>
+      <c r="I93" s="1" t="str">
+        <f>VLOOKUP(B93,Profiled!A$1:A$98,1,FALSE)</f>
+        <v>security.php</v>
       </c>
       <c r="J93" s="1"/>
       <c r="K93" s="1"/>
       <c r="L93" s="1"/>
       <c r="M93" s="1"/>
-      <c r="N93" s="1"/>
-      <c r="O93" s="1"/>
+      <c r="N93" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="O93" s="1" t="s">
+        <v>210</v>
+      </c>
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A94" s="4" t="s">
-        <v>370</v>
-      </c>
       <c r="B94" t="s">
-        <v>194</v>
+        <v>232</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
       <c r="D94" s="1"/>
       <c r="E94" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>211</v>
+        <v>234</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="H94" s="1"/>
-      <c r="I94" s="1" t="str">
-        <f>VLOOKUP(B94,Profiled!A$1:A$98,1,FALSE)</f>
-        <v>session.php</v>
+      <c r="I94" s="1" t="s">
+        <v>271</v>
       </c>
       <c r="J94" s="1"/>
       <c r="K94" s="1"/>
       <c r="L94" s="1"/>
       <c r="M94" s="1"/>
-      <c r="N94" t="s">
-        <v>188</v>
-      </c>
+      <c r="N94" s="1"/>
       <c r="O94" s="1"/>
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.25">
@@ -4189,24 +4208,25 @@
         <v>370</v>
       </c>
       <c r="B95" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>29</v>
       </c>
       <c r="D95" s="1"/>
       <c r="E95" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="H95" s="1"/>
-      <c r="I95" s="1" t="s">
-        <v>271</v>
+      <c r="I95" s="1" t="str">
+        <f>VLOOKUP(B95,Profiled!A$1:A$98,1,FALSE)</f>
+        <v>session.php</v>
       </c>
       <c r="J95" s="1"/>
       <c r="K95" s="1"/>
@@ -4222,7 +4242,7 @@
         <v>370</v>
       </c>
       <c r="B96" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>29</v>
@@ -4232,15 +4252,14 @@
         <v>242</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="H96" s="1"/>
-      <c r="I96" s="1" t="str">
-        <f>VLOOKUP(B96,Profiled!A$1:A$98,1,FALSE)</f>
-        <v>session_delete.php</v>
+      <c r="I96" s="1" t="s">
+        <v>271</v>
       </c>
       <c r="J96" s="1"/>
       <c r="K96" s="1"/>
@@ -4256,7 +4275,7 @@
         <v>370</v>
       </c>
       <c r="B97" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>29</v>
@@ -4266,7 +4285,7 @@
         <v>242</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G97" s="1" t="s">
         <v>224</v>
@@ -4274,7 +4293,7 @@
       <c r="H97" s="1"/>
       <c r="I97" s="1" t="str">
         <f>VLOOKUP(B97,Profiled!A$1:A$98,1,FALSE)</f>
-        <v>session_get.php</v>
+        <v>session_delete.php</v>
       </c>
       <c r="J97" s="1"/>
       <c r="K97" s="1"/>
@@ -4290,7 +4309,7 @@
         <v>370</v>
       </c>
       <c r="B98" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>29</v>
@@ -4300,7 +4319,7 @@
         <v>242</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G98" s="1" t="s">
         <v>224</v>
@@ -4308,7 +4327,7 @@
       <c r="H98" s="1"/>
       <c r="I98" s="1" t="str">
         <f>VLOOKUP(B98,Profiled!A$1:A$98,1,FALSE)</f>
-        <v>session_post.php</v>
+        <v>session_get.php</v>
       </c>
       <c r="J98" s="1"/>
       <c r="K98" s="1"/>
@@ -4324,46 +4343,57 @@
         <v>370</v>
       </c>
       <c r="B99" t="s">
-        <v>248</v>
-      </c>
-      <c r="C99" t="s">
+        <v>198</v>
+      </c>
+      <c r="C99" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E99" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="F99" t="s">
-        <v>260</v>
+      <c r="D99" s="1"/>
+      <c r="E99" t="s">
+        <v>242</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>215</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>222</v>
-      </c>
+        <v>224</v>
+      </c>
+      <c r="H99" s="1"/>
       <c r="I99" s="1" t="str">
         <f>VLOOKUP(B99,Profiled!A$1:A$98,1,FALSE)</f>
-        <v>staff.php</v>
-      </c>
+        <v>session_post.php</v>
+      </c>
+      <c r="J99" s="1"/>
+      <c r="K99" s="1"/>
+      <c r="L99" s="1"/>
+      <c r="M99" s="1"/>
+      <c r="N99" t="s">
+        <v>188</v>
+      </c>
+      <c r="O99" s="1"/>
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
         <v>370</v>
       </c>
       <c r="B100" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C100" t="s">
         <v>29</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F100" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="G100" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="I100" s="1" t="s">
-        <v>271</v>
+      <c r="I100" s="1" t="str">
+        <f>VLOOKUP(B100,Profiled!A$1:A$98,1,FALSE)</f>
+        <v>staff.php</v>
       </c>
     </row>
     <row r="101" spans="1:15" x14ac:dyDescent="0.25">
@@ -4371,7 +4401,7 @@
         <v>370</v>
       </c>
       <c r="B101" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C101" t="s">
         <v>29</v>
@@ -4380,14 +4410,13 @@
         <v>242</v>
       </c>
       <c r="F101" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="I101" s="1" t="str">
-        <f>VLOOKUP(B101,Profiled!A$1:A$98,1,FALSE)</f>
-        <v>staff_get.php</v>
+        <v>222</v>
+      </c>
+      <c r="I101" s="1" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.25">
@@ -4395,7 +4424,7 @@
         <v>370</v>
       </c>
       <c r="B102" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C102" t="s">
         <v>29</v>
@@ -4404,14 +4433,14 @@
         <v>242</v>
       </c>
       <c r="F102" t="s">
-        <v>264</v>
-      </c>
-      <c r="G102" t="s">
-        <v>267</v>
+        <v>265</v>
+      </c>
+      <c r="G102" s="1" t="s">
+        <v>219</v>
       </c>
       <c r="I102" s="1" t="str">
         <f>VLOOKUP(B102,Profiled!A$1:A$98,1,FALSE)</f>
-        <v>staff_patch.php</v>
+        <v>staff_get.php</v>
       </c>
     </row>
     <row r="103" spans="1:15" x14ac:dyDescent="0.25">
@@ -4419,7 +4448,7 @@
         <v>370</v>
       </c>
       <c r="B103" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C103" t="s">
         <v>29</v>
@@ -4428,178 +4457,179 @@
         <v>242</v>
       </c>
       <c r="F103" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="G103" t="s">
         <v>267</v>
       </c>
       <c r="I103" s="1" t="str">
         <f>VLOOKUP(B103,Profiled!A$1:A$98,1,FALSE)</f>
-        <v>staff_post.php</v>
+        <v>staff_patch.php</v>
       </c>
     </row>
     <row r="104" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
-        <v>355</v>
+        <v>370</v>
       </c>
       <c r="B104" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="C104" t="s">
-        <v>31</v>
-      </c>
-      <c r="D104" s="1"/>
+        <v>29</v>
+      </c>
       <c r="E104" s="1" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="F104" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
       <c r="G104" t="s">
-        <v>221</v>
-      </c>
-      <c r="I104" s="1" t="e">
+        <v>267</v>
+      </c>
+      <c r="I104" s="1" t="str">
         <f>VLOOKUP(B104,Profiled!A$1:A$98,1,FALSE)</f>
-        <v>#N/A</v>
+        <v>staff_post.php</v>
       </c>
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="B105" t="s">
+        <v>249</v>
+      </c>
+      <c r="C105" t="s">
+        <v>31</v>
+      </c>
+      <c r="D105" s="1"/>
+      <c r="E105" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="F105" t="s">
+        <v>261</v>
+      </c>
+      <c r="G105" t="s">
+        <v>221</v>
+      </c>
+      <c r="I105" s="1" t="e">
+        <f>VLOOKUP(B105,Profiled!A$1:A$98,1,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A106" s="4" t="s">
         <v>359</v>
       </c>
-      <c r="B105" t="s">
+      <c r="B106" t="s">
         <v>250</v>
       </c>
-      <c r="C105" t="s">
+      <c r="C106" t="s">
         <v>67</v>
-      </c>
-      <c r="E105" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="F105" t="s">
-        <v>262</v>
-      </c>
-      <c r="G105" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="I105" s="1" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B106" t="s">
-        <v>323</v>
-      </c>
-      <c r="C106" t="s">
-        <v>97</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>242</v>
       </c>
       <c r="F106" t="s">
-        <v>339</v>
+        <v>262</v>
       </c>
       <c r="G106" s="1" t="s">
         <v>222</v>
       </c>
+      <c r="I106" s="1" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="107" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
-        <v>334</v>
+        <v>323</v>
       </c>
       <c r="C107" t="s">
-        <v>67</v>
+        <v>97</v>
       </c>
       <c r="E107" s="1" t="s">
         <v>242</v>
       </c>
       <c r="F107" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G107" s="1" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="108" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A108" s="4" t="s">
-        <v>355</v>
-      </c>
       <c r="B108" t="s">
+        <v>334</v>
+      </c>
+      <c r="C108" t="s">
+        <v>67</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="F108" t="s">
+        <v>340</v>
+      </c>
+      <c r="G108" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A109" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="B109" t="s">
         <v>199</v>
       </c>
-      <c r="C108" s="1" t="s">
+      <c r="C109" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D108" s="1"/>
-      <c r="E108" s="1" t="s">
+      <c r="D109" s="1"/>
+      <c r="E109" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="F108" s="1" t="s">
+      <c r="F109" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="G108" s="1" t="s">
+      <c r="G109" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="H108" s="1"/>
-      <c r="I108" s="1" t="str">
-        <f>VLOOKUP(B108,Profiled!A$1:A$98,1,FALSE)</f>
+      <c r="H109" s="1"/>
+      <c r="I109" s="1" t="str">
+        <f>VLOOKUP(B109,Profiled!A$1:A$98,1,FALSE)</f>
         <v>startUiSession.php</v>
       </c>
-      <c r="J108" s="1"/>
-      <c r="K108" s="1"/>
-      <c r="L108" s="1"/>
-      <c r="M108" s="1"/>
-      <c r="N108" t="s">
+      <c r="J109" s="1"/>
+      <c r="K109" s="1"/>
+      <c r="L109" s="1"/>
+      <c r="M109" s="1"/>
+      <c r="N109" t="s">
         <v>188</v>
       </c>
-      <c r="O108" s="1"/>
-    </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B109" t="s">
+      <c r="O109" s="1"/>
+    </row>
+    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B110" t="s">
         <v>344</v>
       </c>
-      <c r="C109" t="s">
+      <c r="C110" t="s">
         <v>97</v>
       </c>
-      <c r="E109" s="1" t="s">
+      <c r="E110" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="F109" t="s">
+      <c r="F110" t="s">
         <v>345</v>
       </c>
-      <c r="G109" s="1" t="s">
+      <c r="G110" s="1" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A110" s="4" t="s">
-        <v>370</v>
-      </c>
-      <c r="B110" t="s">
-        <v>382</v>
-      </c>
-      <c r="C110" t="s">
-        <v>29</v>
-      </c>
-      <c r="D110" s="1"/>
-      <c r="E110" s="1"/>
-      <c r="F110" s="1"/>
-      <c r="G110" s="1"/>
-      <c r="H110" s="1"/>
-      <c r="I110" s="1"/>
-      <c r="J110" s="1"/>
-      <c r="K110" s="1"/>
-      <c r="L110" s="1"/>
-      <c r="M110" s="1"/>
-      <c r="N110" s="1"/>
-      <c r="O110" s="1"/>
     </row>
     <row r="111" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
         <v>370</v>
       </c>
       <c r="B111" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="C111" t="s">
         <v>29</v>
@@ -4622,7 +4652,7 @@
         <v>370</v>
       </c>
       <c r="B112" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="C112" t="s">
         <v>29</v>
@@ -4645,7 +4675,7 @@
         <v>370</v>
       </c>
       <c r="B113" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C113" t="s">
         <v>29</v>
@@ -4668,7 +4698,7 @@
         <v>370</v>
       </c>
       <c r="B114" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C114" t="s">
         <v>29</v>
@@ -4691,7 +4721,7 @@
         <v>370</v>
       </c>
       <c r="B115" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C115" t="s">
         <v>29</v>
@@ -4711,151 +4741,151 @@
     </row>
     <row r="116" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
-        <v>363</v>
+        <v>370</v>
       </c>
       <c r="B116" t="s">
-        <v>108</v>
+        <v>383</v>
       </c>
       <c r="C116" t="s">
-        <v>97</v>
-      </c>
-      <c r="E116" t="s">
-        <v>242</v>
-      </c>
-      <c r="F116" t="s">
-        <v>107</v>
-      </c>
-      <c r="G116" t="s">
-        <v>222</v>
-      </c>
-      <c r="I116" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="N116" t="s">
-        <v>186</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="D116" s="1"/>
+      <c r="E116" s="1"/>
+      <c r="F116" s="1"/>
+      <c r="G116" s="1"/>
+      <c r="H116" s="1"/>
+      <c r="I116" s="1"/>
+      <c r="J116" s="1"/>
+      <c r="K116" s="1"/>
+      <c r="L116" s="1"/>
+      <c r="M116" s="1"/>
+      <c r="N116" s="1"/>
+      <c r="O116" s="1"/>
     </row>
     <row r="117" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
-        <v>355</v>
-      </c>
-      <c r="B117" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C117" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="D117" s="1"/>
-      <c r="E117" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B117" t="s">
+        <v>108</v>
+      </c>
+      <c r="C117" t="s">
+        <v>97</v>
+      </c>
+      <c r="E117" t="s">
         <v>242</v>
       </c>
-      <c r="F117" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="G117" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="H117" s="1" t="s">
+      <c r="F117" t="s">
+        <v>107</v>
+      </c>
+      <c r="G117" t="s">
         <v>222</v>
       </c>
       <c r="I117" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="J117" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="K117" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="L117" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="M117" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="N117" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="O117" s="1" t="s">
-        <v>147</v>
+      <c r="N117" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="118" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
-        <v>359</v>
-      </c>
-      <c r="B118" t="s">
-        <v>98</v>
-      </c>
-      <c r="C118" t="s">
-        <v>67</v>
-      </c>
-      <c r="E118" t="s">
+        <v>355</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D118" s="1"/>
+      <c r="E118" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="F118" t="s">
-        <v>99</v>
+      <c r="F118" s="1" t="s">
+        <v>237</v>
       </c>
       <c r="G118" s="1" t="s">
         <v>222</v>
       </c>
+      <c r="H118" s="1" t="s">
+        <v>222</v>
+      </c>
       <c r="I118" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="N118" t="s">
-        <v>164</v>
-      </c>
-      <c r="O118" t="s">
-        <v>157</v>
+      <c r="J118" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="K118" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="L118" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="M118" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="N118" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="O118" s="1" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="119" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="B119" t="s">
-        <v>233</v>
-      </c>
-      <c r="C119" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="D119" s="1"/>
-      <c r="E119" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C119" t="s">
+        <v>67</v>
+      </c>
+      <c r="E119" t="s">
         <v>242</v>
       </c>
-      <c r="F119" s="1" t="s">
-        <v>235</v>
+      <c r="F119" t="s">
+        <v>99</v>
       </c>
       <c r="G119" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="H119" s="1"/>
       <c r="I119" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="J119" s="1"/>
-      <c r="K119" s="1"/>
-      <c r="L119" s="1"/>
-      <c r="M119" s="1"/>
-      <c r="N119" s="1"/>
-      <c r="O119" s="1"/>
+      <c r="N119" t="s">
+        <v>164</v>
+      </c>
+      <c r="O119" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="120" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="B120" t="s">
-        <v>361</v>
+        <v>233</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>67</v>
+        <v>223</v>
       </c>
       <c r="D120" s="1"/>
-      <c r="E120" s="1"/>
-      <c r="F120" s="1"/>
-      <c r="G120" s="1"/>
+      <c r="E120" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="F120" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="G120" s="1" t="s">
+        <v>222</v>
+      </c>
       <c r="H120" s="1"/>
-      <c r="I120" s="1"/>
+      <c r="I120" s="1" t="s">
+        <v>271</v>
+      </c>
       <c r="J120" s="1"/>
       <c r="K120" s="1"/>
       <c r="L120" s="1"/>
@@ -4863,99 +4893,95 @@
       <c r="N120" s="1"/>
       <c r="O120" s="1"/>
     </row>
-    <row r="121" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="B121" s="1" t="s">
-        <v>20</v>
+    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A121" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="B121" t="s">
+        <v>361</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>30</v>
+        <v>67</v>
       </c>
       <c r="D121" s="1"/>
-      <c r="E121" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="F121" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="G121" s="1" t="s">
-        <v>221</v>
-      </c>
+      <c r="E121" s="1"/>
+      <c r="F121" s="1"/>
+      <c r="G121" s="1"/>
       <c r="H121" s="1"/>
-      <c r="I121" s="1" t="e">
-        <f>VLOOKUP(B121,Profiled!A$1:A$98,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
+      <c r="I121" s="1"/>
       <c r="J121" s="1"/>
       <c r="K121" s="1"/>
       <c r="L121" s="1"/>
       <c r="M121" s="1"/>
-      <c r="N121" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="O121" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B122" t="s">
-        <v>292</v>
-      </c>
-      <c r="C122" t="s">
-        <v>31</v>
+      <c r="N121" s="1"/>
+      <c r="O121" s="1"/>
+    </row>
+    <row r="122" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="B122" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="D122" s="1"/>
       <c r="E122" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="F122" t="s">
-        <v>303</v>
+        <v>241</v>
+      </c>
+      <c r="F122" s="1" t="s">
+        <v>100</v>
       </c>
       <c r="G122" s="1" t="s">
         <v>221</v>
       </c>
+      <c r="H122" s="1"/>
+      <c r="I122" s="1" t="e">
+        <f>VLOOKUP(B122,Profiled!A$1:A$98,1,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J122" s="1"/>
+      <c r="K122" s="1"/>
+      <c r="L122" s="1"/>
+      <c r="M122" s="1"/>
+      <c r="N122" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="O122" s="2" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="123" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
+        <v>292</v>
+      </c>
+      <c r="C123" t="s">
+        <v>31</v>
+      </c>
+      <c r="D123" s="1"/>
+      <c r="E123" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="F123" t="s">
+        <v>303</v>
+      </c>
+      <c r="G123" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B124" t="s">
         <v>293</v>
       </c>
-      <c r="C123" t="s">
+      <c r="C124" t="s">
         <v>67</v>
       </c>
-      <c r="E123" t="s">
+      <c r="E124" t="s">
         <v>242</v>
       </c>
-      <c r="F123" t="s">
+      <c r="F124" t="s">
         <v>304</v>
-      </c>
-      <c r="G123" s="1" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A124" s="4" t="s">
-        <v>370</v>
-      </c>
-      <c r="B124" t="s">
-        <v>21</v>
-      </c>
-      <c r="C124" t="s">
-        <v>29</v>
-      </c>
-      <c r="E124" t="s">
-        <v>241</v>
-      </c>
-      <c r="F124" t="s">
-        <v>58</v>
       </c>
       <c r="G124" s="1" t="s">
         <v>222</v>
-      </c>
-      <c r="I124" s="1" t="str">
-        <f>VLOOKUP(B124,Profiled!A$1:A$98,1,FALSE)</f>
-        <v>visit.php</v>
-      </c>
-      <c r="N124" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="125" spans="1:15" x14ac:dyDescent="0.25">
@@ -4963,22 +4989,23 @@
         <v>370</v>
       </c>
       <c r="B125" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C125" t="s">
         <v>29</v>
       </c>
       <c r="E125" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F125" t="s">
-        <v>101</v>
+        <v>58</v>
       </c>
       <c r="G125" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="I125" s="1" t="s">
-        <v>271</v>
+      <c r="I125" s="1" t="str">
+        <f>VLOOKUP(B125,Profiled!A$1:A$98,1,FALSE)</f>
+        <v>visit.php</v>
       </c>
       <c r="N125" t="s">
         <v>185</v>
@@ -4989,7 +5016,7 @@
         <v>370</v>
       </c>
       <c r="B126" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C126" t="s">
         <v>29</v>
@@ -4998,17 +5025,16 @@
         <v>242</v>
       </c>
       <c r="F126" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G126" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="I126" s="1" t="str">
-        <f>VLOOKUP(B126,Profiled!A$1:A$98,1,FALSE)</f>
-        <v>visit_get.php</v>
+        <v>222</v>
+      </c>
+      <c r="I126" s="1" t="s">
+        <v>271</v>
       </c>
       <c r="N126" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="127" spans="1:15" x14ac:dyDescent="0.25">
@@ -5016,7 +5042,7 @@
         <v>370</v>
       </c>
       <c r="B127" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C127" t="s">
         <v>29</v>
@@ -5025,14 +5051,14 @@
         <v>242</v>
       </c>
       <c r="F127" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="G127" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I127" s="1" t="str">
         <f>VLOOKUP(B127,Profiled!A$1:A$98,1,FALSE)</f>
-        <v>visit_patch.php</v>
+        <v>visit_get.php</v>
       </c>
       <c r="N127" t="s">
         <v>188</v>
@@ -5043,7 +5069,7 @@
         <v>370</v>
       </c>
       <c r="B128" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C128" t="s">
         <v>29</v>
@@ -5052,324 +5078,351 @@
         <v>242</v>
       </c>
       <c r="F128" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G128" s="1" t="s">
         <v>221</v>
       </c>
       <c r="I128" s="1" t="str">
         <f>VLOOKUP(B128,Profiled!A$1:A$98,1,FALSE)</f>
-        <v>visit_post.php</v>
+        <v>visit_patch.php</v>
       </c>
       <c r="N128" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="129" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B129" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C129" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D129" s="1"/>
-      <c r="E129" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="F129" s="1" t="s">
-        <v>39</v>
+    <row r="129" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A129" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="B129" t="s">
+        <v>25</v>
+      </c>
+      <c r="C129" t="s">
+        <v>29</v>
+      </c>
+      <c r="E129" t="s">
+        <v>242</v>
+      </c>
+      <c r="F129" t="s">
+        <v>103</v>
       </c>
       <c r="G129" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="H129" s="1" t="s">
+      <c r="I129" s="1" t="str">
+        <f>VLOOKUP(B129,Profiled!A$1:A$98,1,FALSE)</f>
+        <v>visit_post.php</v>
+      </c>
+      <c r="N129" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="130" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B130" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D130" s="1"/>
+      <c r="E130" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="F130" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G130" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="H130" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="I129" s="1" t="e">
-        <f>VLOOKUP(B129,Profiled!A$1:A$98,1,FALSE)</f>
+      <c r="I130" s="1" t="e">
+        <f>VLOOKUP(B130,Profiled!A$1:A$98,1,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="J129" s="1"/>
-      <c r="K129" s="1" t="s">
+      <c r="J130" s="1"/>
+      <c r="K130" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="L129" s="1" t="s">
+      <c r="L130" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="M129" s="1" t="s">
+      <c r="M130" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="N129" s="1" t="s">
+      <c r="N130" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="O129" s="1" t="s">
+      <c r="O130" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="130" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B130" t="s">
+    <row r="131" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B131" t="s">
         <v>75</v>
       </c>
-      <c r="C130" t="s">
+      <c r="C131" t="s">
         <v>67</v>
       </c>
-      <c r="E130" t="s">
+      <c r="E131" t="s">
         <v>242</v>
       </c>
-      <c r="F130" t="s">
+      <c r="F131" t="s">
         <v>84</v>
       </c>
-      <c r="G130" s="1" t="s">
+      <c r="G131" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="I130" s="1" t="s">
+      <c r="I131" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="N130" t="s">
+      <c r="N131" t="s">
         <v>165</v>
       </c>
-      <c r="O130" t="s">
+      <c r="O131" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="131" spans="2:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="B131" s="1" t="s">
+    <row r="132" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="B132" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C131" s="1" t="s">
+      <c r="C132" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D131" s="1"/>
-      <c r="E131" s="1" t="s">
+      <c r="D132" s="1"/>
+      <c r="E132" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="F131" s="1" t="s">
+      <c r="F132" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="G131" s="1" t="s">
+      <c r="G132" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="H131" s="1" t="s">
+      <c r="H132" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="I131" s="1" t="e">
-        <f>VLOOKUP(B131,Profiled!A$1:A$98,1,FALSE)</f>
+      <c r="I132" s="1" t="e">
+        <f>VLOOKUP(B132,Profiled!A$1:A$98,1,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="J131" s="1"/>
-      <c r="K131" s="1" t="s">
+      <c r="J132" s="1"/>
+      <c r="K132" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="L131" s="1" t="s">
+      <c r="L132" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="M131" s="1" t="s">
+      <c r="M132" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="N131" s="2" t="s">
+      <c r="N132" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="O131" s="2" t="s">
+      <c r="O132" s="2" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="132" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B132" t="s">
+    <row r="133" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B133" t="s">
         <v>76</v>
       </c>
-      <c r="C132" t="s">
+      <c r="C133" t="s">
         <v>67</v>
       </c>
-      <c r="E132" t="s">
+      <c r="E133" t="s">
         <v>242</v>
       </c>
-      <c r="F132" t="s">
+      <c r="F133" t="s">
         <v>85</v>
       </c>
-      <c r="G132" s="1" t="s">
+      <c r="G133" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="I132" s="1" t="s">
+      <c r="I133" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="N132" t="s">
+      <c r="N133" t="s">
         <v>168</v>
       </c>
-      <c r="O132" t="s">
+      <c r="O133" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="133" spans="2:15" ht="90" x14ac:dyDescent="0.25">
-      <c r="B133" s="1" t="s">
+    <row r="134" spans="1:15" ht="90" x14ac:dyDescent="0.25">
+      <c r="B134" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C133" s="1" t="s">
+      <c r="C134" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D133" s="1"/>
-      <c r="E133" s="1" t="s">
+      <c r="D134" s="1"/>
+      <c r="E134" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="F133" s="1" t="s">
+      <c r="F134" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="G133" s="1" t="s">
+      <c r="G134" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="H133" s="1" t="s">
+      <c r="H134" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="I133" s="1" t="e">
-        <f>VLOOKUP(B133,Profiled!A$1:A$98,1,FALSE)</f>
+      <c r="I134" s="1" t="e">
+        <f>VLOOKUP(B134,Profiled!A$1:A$98,1,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="J133" s="1"/>
-      <c r="K133" s="1" t="s">
+      <c r="J134" s="1"/>
+      <c r="K134" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="L133" s="1" t="s">
+      <c r="L134" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="M133" s="1" t="s">
+      <c r="M134" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="N133" s="2" t="s">
+      <c r="N134" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="O133" s="2" t="s">
+      <c r="O134" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="134" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B134" t="s">
+    <row r="135" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B135" t="s">
         <v>77</v>
       </c>
-      <c r="C134" t="s">
+      <c r="C135" t="s">
         <v>67</v>
       </c>
-      <c r="E134" t="s">
+      <c r="E135" t="s">
         <v>242</v>
       </c>
-      <c r="F134" t="s">
+      <c r="F135" t="s">
         <v>86</v>
       </c>
-      <c r="G134" s="1" t="s">
+      <c r="G135" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="I134" s="1" t="s">
+      <c r="I135" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="N134" t="s">
+      <c r="N135" t="s">
         <v>169</v>
       </c>
-      <c r="O134" t="s">
+      <c r="O135" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="135" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B135" t="s">
+    <row r="136" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B136" t="s">
         <v>95</v>
       </c>
-      <c r="C135" t="s">
+      <c r="C136" t="s">
         <v>31</v>
       </c>
-      <c r="D135" s="1"/>
-      <c r="E135" s="1" t="s">
+      <c r="D136" s="1"/>
+      <c r="E136" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="F135" t="s">
+      <c r="F136" t="s">
         <v>48</v>
       </c>
-      <c r="G135" s="1" t="s">
+      <c r="G136" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="H135" s="1" t="s">
+      <c r="H136" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="I135" s="1" t="e">
-        <f>VLOOKUP(B135,Profiled!A$1:A$98,1,FALSE)</f>
+      <c r="I136" s="1" t="e">
+        <f>VLOOKUP(B136,Profiled!A$1:A$98,1,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="K135" s="1" t="s">
+      <c r="K136" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="L135" s="1" t="s">
+      <c r="L136" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="M135" s="1" t="s">
+      <c r="M136" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="N135" s="1" t="s">
+      <c r="N136" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="O135" s="1" t="s">
+      <c r="O136" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="136" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B136" t="s">
+    <row r="137" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B137" t="s">
         <v>78</v>
       </c>
-      <c r="C136" t="s">
+      <c r="C137" t="s">
         <v>67</v>
       </c>
-      <c r="E136" t="s">
+      <c r="E137" t="s">
         <v>242</v>
       </c>
-      <c r="F136" t="s">
+      <c r="F137" t="s">
         <v>87</v>
-      </c>
-      <c r="G136" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="I136" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="N136" t="s">
-        <v>170</v>
-      </c>
-      <c r="O136" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="137" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B137" t="s">
-        <v>335</v>
-      </c>
-      <c r="C137" t="s">
-        <v>97</v>
-      </c>
-      <c r="E137" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="F137" t="s">
-        <v>341</v>
       </c>
       <c r="G137" s="1" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="138" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="I137" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="N137" t="s">
+        <v>170</v>
+      </c>
+      <c r="O137" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="138" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B138" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C138" t="s">
-        <v>67</v>
+        <v>97</v>
       </c>
       <c r="E138" s="1" t="s">
         <v>242</v>
       </c>
       <c r="F138" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G138" s="1" t="s">
         <v>222</v>
       </c>
     </row>
+    <row r="139" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B139" t="s">
+        <v>336</v>
+      </c>
+      <c r="C139" t="s">
+        <v>67</v>
+      </c>
+      <c r="E139" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="F139" t="s">
+        <v>342</v>
+      </c>
+      <c r="G139" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:O138">
-    <sortState ref="A2:O138">
-      <sortCondition ref="B1:B138"/>
+  <autoFilter ref="A1:O139">
+    <sortState ref="A2:O139">
+      <sortCondition ref="B1:B139"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added user comment UI
</commit_message>
<xml_diff>
--- a/tools/web file descriptions.xlsx
+++ b/tools/web file descriptions.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1272" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1276" uniqueCount="389">
   <si>
     <t>addPatient.php</t>
   </si>
@@ -1584,17 +1584,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:O139"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:G1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="4"/>
     <col min="2" max="2" width="29" customWidth="1"/>
-    <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="4" max="5" width="10" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="43.85546875" hidden="1" customWidth="1"/>
+    <col min="3" max="5" width="10" customWidth="1"/>
+    <col min="6" max="6" width="43.85546875" customWidth="1"/>
     <col min="7" max="7" width="44.42578125" customWidth="1"/>
     <col min="8" max="13" width="20.7109375" customWidth="1"/>
     <col min="14" max="14" width="36" customWidth="1"/>
@@ -1645,8 +1647,10 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
+    <row r="2" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>386</v>
+      </c>
       <c r="B2" t="s">
         <v>282</v>
       </c>
@@ -1670,7 +1674,7 @@
       <c r="N2"/>
       <c r="O2"/>
     </row>
-    <row r="3" spans="1:15" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>386</v>
       </c>
@@ -1700,7 +1704,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="4" spans="1:15" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" s="1" customFormat="1" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>384</v>
       </c>
@@ -1763,7 +1767,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>386</v>
       </c>
@@ -1795,7 +1799,7 @@
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>355</v>
       </c>
@@ -1827,7 +1831,7 @@
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
     </row>
-    <row r="8" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>359</v>
       </c>
@@ -1893,7 +1897,10 @@
         <v>222</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>384</v>
+      </c>
       <c r="B11" t="s">
         <v>62</v>
       </c>
@@ -2001,7 +2008,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>370</v>
       </c>
@@ -2027,7 +2034,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>355</v>
       </c>
@@ -2042,7 +2049,7 @@
       </c>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>359</v>
       </c>
@@ -2112,7 +2119,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>370</v>
       </c>
@@ -2135,7 +2142,7 @@
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>370</v>
       </c>
@@ -2158,7 +2165,7 @@
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>370</v>
       </c>
@@ -2181,7 +2188,7 @@
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
     </row>
-    <row r="25" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>355</v>
       </c>
@@ -2225,7 +2232,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>359</v>
       </c>
@@ -2254,7 +2261,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>355</v>
       </c>
@@ -2300,7 +2307,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>359</v>
       </c>
@@ -2335,7 +2342,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>355</v>
       </c>
@@ -2361,7 +2368,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>370</v>
       </c>
@@ -2381,7 +2388,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>370</v>
       </c>
@@ -2401,7 +2408,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="32" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>370</v>
       </c>
@@ -2430,7 +2437,7 @@
       <c r="N32"/>
       <c r="O32"/>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>370</v>
       </c>
@@ -2450,7 +2457,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="34" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>385</v>
       </c>
@@ -2483,7 +2490,7 @@
       </c>
       <c r="O34"/>
     </row>
-    <row r="35" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>363</v>
       </c>
@@ -2516,7 +2523,7 @@
       </c>
       <c r="O35"/>
     </row>
-    <row r="36" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>384</v>
       </c>
@@ -2552,7 +2559,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="37" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>386</v>
       </c>
@@ -2582,7 +2589,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="38" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>355</v>
       </c>
@@ -2609,7 +2616,7 @@
       <c r="N38"/>
       <c r="O38"/>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>363</v>
       </c>
@@ -2629,7 +2636,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="40" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>355</v>
       </c>
@@ -2657,7 +2664,7 @@
       <c r="N40"/>
       <c r="O40"/>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>359</v>
       </c>
@@ -2677,7 +2684,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="42" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>370</v>
       </c>
@@ -2706,7 +2713,7 @@
       <c r="N42"/>
       <c r="O42"/>
     </row>
-    <row r="43" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>370</v>
       </c>
@@ -2735,7 +2742,7 @@
       <c r="N43"/>
       <c r="O43"/>
     </row>
-    <row r="44" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>370</v>
       </c>
@@ -2764,7 +2771,7 @@
       <c r="N44"/>
       <c r="O44"/>
     </row>
-    <row r="45" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>370</v>
       </c>
@@ -2793,7 +2800,7 @@
       <c r="N45"/>
       <c r="O45"/>
     </row>
-    <row r="46" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>369</v>
       </c>
@@ -2822,7 +2829,7 @@
       <c r="N46"/>
       <c r="O46"/>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>384</v>
       </c>
@@ -2849,7 +2856,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>384</v>
       </c>
@@ -2875,7 +2882,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>384</v>
       </c>
@@ -2902,7 +2909,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="50" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>384</v>
       </c>
@@ -2936,7 +2943,7 @@
       </c>
       <c r="O50"/>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>384</v>
       </c>
@@ -2963,7 +2970,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="52" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>384</v>
       </c>
@@ -2997,7 +3004,7 @@
       </c>
       <c r="O52"/>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>384</v>
       </c>
@@ -3024,7 +3031,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>355</v>
       </c>
@@ -3038,7 +3045,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>370</v>
       </c>
@@ -3051,7 +3058,7 @@
       <c r="G55" s="1"/>
       <c r="I55" s="1"/>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>370</v>
       </c>
@@ -3064,7 +3071,7 @@
       <c r="G56" s="1"/>
       <c r="I56" s="1"/>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>370</v>
       </c>
@@ -3077,7 +3084,7 @@
       <c r="G57" s="1"/>
       <c r="I57" s="1"/>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>370</v>
       </c>
@@ -3090,7 +3097,7 @@
       <c r="G58" s="1"/>
       <c r="I58" s="1"/>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>363</v>
       </c>
@@ -3102,7 +3109,7 @@
       </c>
       <c r="G59" s="1"/>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>384</v>
       </c>
@@ -3133,7 +3140,7 @@
       <c r="N60" s="1"/>
       <c r="O60" s="1"/>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>370</v>
       </c>
@@ -3160,7 +3167,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="62" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>370</v>
       </c>
@@ -3193,7 +3200,7 @@
       </c>
       <c r="O62"/>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>370</v>
       </c>
@@ -3220,7 +3227,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="64" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>370</v>
       </c>
@@ -3254,7 +3261,7 @@
       </c>
       <c r="O64"/>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>370</v>
       </c>
@@ -3281,7 +3288,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="66" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>370</v>
       </c>
@@ -3315,7 +3322,7 @@
       </c>
       <c r="O66"/>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>355</v>
       </c>
@@ -3341,7 +3348,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>366</v>
       </c>
@@ -3361,7 +3368,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>363</v>
       </c>
@@ -3387,7 +3394,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="70" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>363</v>
       </c>
@@ -3418,7 +3425,7 @@
       <c r="N70"/>
       <c r="O70"/>
     </row>
-    <row r="71" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
         <v>355</v>
       </c>
@@ -3460,7 +3467,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="72" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>359</v>
       </c>
@@ -3495,7 +3502,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="73" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>384</v>
       </c>
@@ -3537,7 +3544,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="74" spans="1:15" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" s="1" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>384</v>
       </c>
@@ -3579,7 +3586,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="75" spans="1:15" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" s="1" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
         <v>384</v>
       </c>
@@ -3608,7 +3615,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="76" spans="1:15" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" s="1" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
         <v>355</v>
       </c>
@@ -3649,7 +3656,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="77" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
         <v>359</v>
       </c>
@@ -3684,7 +3691,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="78" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>355</v>
       </c>
@@ -3726,7 +3733,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="79" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
         <v>359</v>
       </c>
@@ -3761,7 +3768,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="80" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>384</v>
       </c>
@@ -3803,7 +3810,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="81" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>384</v>
       </c>
@@ -3838,7 +3845,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="82" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
         <v>384</v>
       </c>
@@ -3877,7 +3884,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="83" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
         <v>355</v>
       </c>
@@ -3919,7 +3926,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="84" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
         <v>359</v>
       </c>
@@ -4139,7 +4146,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
         <v>363</v>
       </c>
@@ -4203,7 +4210,7 @@
       <c r="N94" s="1"/>
       <c r="O94" s="1"/>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
         <v>370</v>
       </c>
@@ -4237,7 +4244,7 @@
       </c>
       <c r="O95" s="1"/>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
         <v>370</v>
       </c>
@@ -4270,7 +4277,7 @@
       </c>
       <c r="O96" s="1"/>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
         <v>370</v>
       </c>
@@ -4304,7 +4311,7 @@
       </c>
       <c r="O97" s="1"/>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
         <v>370</v>
       </c>
@@ -4338,7 +4345,7 @@
       </c>
       <c r="O98" s="1"/>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
         <v>370</v>
       </c>
@@ -4372,7 +4379,7 @@
       </c>
       <c r="O99" s="1"/>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
         <v>370</v>
       </c>
@@ -4396,7 +4403,7 @@
         <v>staff.php</v>
       </c>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
         <v>370</v>
       </c>
@@ -4419,7 +4426,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
         <v>370</v>
       </c>
@@ -4443,7 +4450,7 @@
         <v>staff_get.php</v>
       </c>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
         <v>370</v>
       </c>
@@ -4467,7 +4474,7 @@
         <v>staff_patch.php</v>
       </c>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
         <v>370</v>
       </c>
@@ -4491,7 +4498,7 @@
         <v>staff_post.php</v>
       </c>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
         <v>355</v>
       </c>
@@ -4516,7 +4523,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
         <v>359</v>
       </c>
@@ -4573,7 +4580,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
         <v>386</v>
       </c>
@@ -4624,7 +4631,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
         <v>370</v>
       </c>
@@ -4647,7 +4654,7 @@
       <c r="N111" s="1"/>
       <c r="O111" s="1"/>
     </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
         <v>370</v>
       </c>
@@ -4670,7 +4677,7 @@
       <c r="N112" s="1"/>
       <c r="O112" s="1"/>
     </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
         <v>370</v>
       </c>
@@ -4693,7 +4700,7 @@
       <c r="N113" s="1"/>
       <c r="O113" s="1"/>
     </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
         <v>370</v>
       </c>
@@ -4716,7 +4723,7 @@
       <c r="N114" s="1"/>
       <c r="O114" s="1"/>
     </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
         <v>370</v>
       </c>
@@ -4739,7 +4746,7 @@
       <c r="N115" s="1"/>
       <c r="O115" s="1"/>
     </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
         <v>370</v>
       </c>
@@ -4762,7 +4769,7 @@
       <c r="N116" s="1"/>
       <c r="O116" s="1"/>
     </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
         <v>363</v>
       </c>
@@ -4788,7 +4795,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
         <v>355</v>
       </c>
@@ -4833,7 +4840,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
         <v>359</v>
       </c>
@@ -4862,7 +4869,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
         <v>355</v>
       </c>
@@ -4893,7 +4900,7 @@
       <c r="N120" s="1"/>
       <c r="O120" s="1"/>
     </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="4" t="s">
         <v>359</v>
       </c>
@@ -4949,7 +4956,10 @@
         <v>179</v>
       </c>
     </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="4" t="s">
+        <v>355</v>
+      </c>
       <c r="B123" t="s">
         <v>292</v>
       </c>
@@ -4967,7 +4977,10 @@
         <v>221</v>
       </c>
     </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="4" t="s">
+        <v>359</v>
+      </c>
       <c r="B124" t="s">
         <v>293</v>
       </c>
@@ -4984,7 +4997,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="s">
         <v>370</v>
       </c>
@@ -5011,7 +5024,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="4" t="s">
         <v>370</v>
       </c>
@@ -5037,7 +5050,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="4" t="s">
         <v>370</v>
       </c>
@@ -5064,7 +5077,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="4" t="s">
         <v>370</v>
       </c>
@@ -5091,7 +5104,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="129" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="4" t="s">
         <v>370</v>
       </c>
@@ -5421,6 +5434,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:O139">
+    <filterColumn colId="0">
+      <filters blank="1"/>
+    </filterColumn>
     <sortState ref="A2:O139">
       <sortCondition ref="B1:B139"/>
     </sortState>

</xml_diff>

<commit_message>
updated to match current state of the project
</commit_message>
<xml_diff>
--- a/tools/web file descriptions.xlsx
+++ b/tools/web file descriptions.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1287" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1290" uniqueCount="389">
   <si>
     <t>addPatient.php</t>
   </si>
@@ -1588,7 +1588,7 @@
   <dimension ref="A1:O139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A136" sqref="A136"/>
+      <selection activeCell="A110" sqref="A110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2197,10 +2197,7 @@
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
     </row>
-    <row r="25" spans="1:15" ht="75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>355</v>
-      </c>
+    <row r="25" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>65</v>
       </c>
@@ -5146,7 +5143,10 @@
         <v>188</v>
       </c>
     </row>
-    <row r="130" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="4" t="s">
+        <v>355</v>
+      </c>
       <c r="B130" s="1" t="s">
         <v>92</v>
       </c>
@@ -5187,7 +5187,10 @@
         <v>149</v>
       </c>
     </row>
-    <row r="131" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="4" t="s">
+        <v>359</v>
+      </c>
       <c r="B131" t="s">
         <v>75</v>
       </c>
@@ -5359,7 +5362,10 @@
         <v>157</v>
       </c>
     </row>
-    <row r="136" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="4" t="s">
+        <v>355</v>
+      </c>
       <c r="B136" t="s">
         <v>95</v>
       </c>
@@ -5399,7 +5405,10 @@
         <v>155</v>
       </c>
     </row>
-    <row r="137" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="4" t="s">
+        <v>359</v>
+      </c>
       <c r="B137" t="s">
         <v>78</v>
       </c>

</xml_diff>

<commit_message>
Working on tagging links
</commit_message>
<xml_diff>
--- a/tools/web file descriptions.xlsx
+++ b/tools/web file descriptions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="90" windowWidth="20730" windowHeight="11760" tabRatio="388"/>
+    <workbookView xWindow="480" yWindow="90" windowWidth="20730" windowHeight="11760" tabRatio="388" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Current" sheetId="2" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Profiled" sheetId="4" r:id="rId3"/>
     <sheet name="Sheet2" sheetId="5" r:id="rId4"/>
     <sheet name="Sheet3" sheetId="6" r:id="rId5"/>
+    <sheet name="Workflows" sheetId="7" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Current!$A$1:$O$139</definedName>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1298" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1333" uniqueCount="402">
   <si>
     <t>addPatient.php</t>
   </si>
@@ -1233,10 +1234,40 @@
     <t>reports</t>
   </si>
   <si>
-    <t>reports/uitext</t>
-  </si>
-  <si>
     <t>support</t>
+  </si>
+  <si>
+    <t>reports\uitext</t>
+  </si>
+  <si>
+    <t>Workflow\screen</t>
+  </si>
+  <si>
+    <t>AdmitPatient</t>
+  </si>
+  <si>
+    <t>Step</t>
+  </si>
+  <si>
+    <t>Step/End</t>
+  </si>
+  <si>
+    <t>DischargePatient</t>
+  </si>
+  <si>
+    <t>Start (searchbox)</t>
+  </si>
+  <si>
+    <t>Start (listLink)</t>
+  </si>
+  <si>
+    <t>Start (status link)</t>
+  </si>
+  <si>
+    <t>EditPatient</t>
+  </si>
+  <si>
+    <t>Start (edit link)</t>
   </si>
 </sst>
 </file>
@@ -1280,7 +1311,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1291,6 +1322,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1596,8 +1631,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:O139"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A90" sqref="A90"/>
+    <sheetView topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:B136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1811,7 +1846,7 @@
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
     </row>
-    <row r="7" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>355</v>
       </c>
@@ -1892,7 +1927,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>273</v>
       </c>
@@ -1951,7 +1986,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="13" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" t="s">
         <v>284</v>
@@ -2000,7 +2035,7 @@
         <v>adminShowUsers.php</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>247</v>
       </c>
@@ -2046,7 +2081,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="17" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>355</v>
       </c>
@@ -2209,7 +2244,7 @@
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
     </row>
-    <row r="25" spans="1:15" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>355</v>
       </c>
@@ -2282,7 +2317,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>355</v>
       </c>
@@ -2610,7 +2645,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="38" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>355</v>
       </c>
@@ -2657,7 +2692,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="40" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>355</v>
       </c>
@@ -3052,7 +3087,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="54" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>355</v>
       </c>
@@ -3446,7 +3481,7 @@
       <c r="N70"/>
       <c r="O70"/>
     </row>
-    <row r="71" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
         <v>355</v>
       </c>
@@ -3636,7 +3671,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="76" spans="1:15" s="1" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
         <v>355</v>
       </c>
@@ -3712,7 +3747,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="78" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>355</v>
       </c>
@@ -3905,7 +3940,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="83" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
         <v>355</v>
       </c>
@@ -4022,7 +4057,7 @@
     </row>
     <row r="86" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>112</v>
@@ -4078,7 +4113,7 @@
     </row>
     <row r="88" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B88" t="s">
         <v>348</v>
@@ -4117,7 +4152,10 @@
         <v>220</v>
       </c>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="4" t="s">
+        <v>389</v>
+      </c>
       <c r="B90" t="s">
         <v>308</v>
       </c>
@@ -4159,7 +4197,10 @@
         <v>220</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="4" t="s">
+        <v>391</v>
+      </c>
       <c r="B92" t="s">
         <v>309</v>
       </c>
@@ -4537,7 +4578,7 @@
         <v>staff_post.php</v>
       </c>
     </row>
-    <row r="105" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
         <v>355</v>
       </c>
@@ -4585,7 +4626,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
         <v>323</v>
       </c>
@@ -4602,7 +4643,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
         <v>334</v>
       </c>
@@ -4655,7 +4696,7 @@
     </row>
     <row r="110" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B110" t="s">
         <v>344</v>
@@ -5001,7 +5042,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="123" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A123" s="4" t="s">
         <v>355</v>
       </c>
@@ -5176,7 +5217,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="130" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="s">
         <v>355</v>
       </c>
@@ -5249,7 +5290,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="132" spans="1:15" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A132" s="4" t="s">
         <v>355</v>
       </c>
@@ -5322,7 +5363,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="134" spans="1:15" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:15" ht="90" x14ac:dyDescent="0.25">
       <c r="A134" s="4" t="s">
         <v>355</v>
       </c>
@@ -5395,7 +5436,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="136" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A136" s="4" t="s">
         <v>355</v>
       </c>
@@ -5510,7 +5551,14 @@
   </sheetData>
   <autoFilter ref="A1:O139">
     <filterColumn colId="0">
-      <filters blank="1"/>
+      <filters blank="1">
+        <filter val="root"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="2">
+      <filters>
+        <filter val="UI"/>
+      </filters>
     </filterColumn>
     <sortState ref="A2:O139">
       <sortCondition ref="B1:B139"/>
@@ -8077,4 +8125,149 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>392</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>357</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>358</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>343</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="T1" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>393</v>
+      </c>
+      <c r="G2" t="s">
+        <v>397</v>
+      </c>
+      <c r="K2" t="s">
+        <v>394</v>
+      </c>
+      <c r="M2" t="s">
+        <v>394</v>
+      </c>
+      <c r="U2" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>396</v>
+      </c>
+      <c r="G3" t="s">
+        <v>398</v>
+      </c>
+      <c r="L3" t="s">
+        <v>399</v>
+      </c>
+      <c r="R3" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>400</v>
+      </c>
+      <c r="K4" t="s">
+        <v>395</v>
+      </c>
+      <c r="L4" t="s">
+        <v>401</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added notes for how to get the workflow data back
</commit_message>
<xml_diff>
--- a/tools/web file descriptions.xlsx
+++ b/tools/web file descriptions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="90" windowWidth="20730" windowHeight="11760" tabRatio="388" activeTab="5"/>
+    <workbookView xWindow="480" yWindow="90" windowWidth="20730" windowHeight="11760" tabRatio="388"/>
   </bookViews>
   <sheets>
     <sheet name="Current" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1333" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1334" uniqueCount="403">
   <si>
     <t>addPatient.php</t>
   </si>
@@ -1268,6 +1268,9 @@
   </si>
   <si>
     <t>Start (edit link)</t>
+  </si>
+  <si>
+    <t>Add Patient</t>
   </si>
 </sst>
 </file>
@@ -1631,7 +1634,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:O139"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
@@ -5551,7 +5554,7 @@
   </sheetData>
   <autoFilter ref="A1:O139">
     <filterColumn colId="0">
-      <filters blank="1">
+      <filters>
         <filter val="root"/>
       </filters>
     </filterColumn>
@@ -8129,10 +8132,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U4"/>
+  <dimension ref="A1:U5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8266,6 +8269,11 @@
         <v>401</v>
       </c>
     </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>402</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Added log viewer (start)
The log viewer is a work in progress, still.
</commit_message>
<xml_diff>
--- a/tools/web file descriptions.xlsx
+++ b/tools/web file descriptions.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1334" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1343" uniqueCount="403">
   <si>
     <t>addPatient.php</t>
   </si>
@@ -1631,11 +1631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:O139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="A108" sqref="A108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1694,7 +1693,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>386</v>
       </c>
@@ -1721,7 +1720,7 @@
       <c r="N2"/>
       <c r="O2"/>
     </row>
-    <row r="3" spans="1:15" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>386</v>
       </c>
@@ -1751,7 +1750,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="4" spans="1:15" s="1" customFormat="1" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>384</v>
       </c>
@@ -1781,7 +1780,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="5" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>386</v>
       </c>
@@ -1817,7 +1816,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="6" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>386</v>
       </c>
@@ -1881,7 +1880,7 @@
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
     </row>
-    <row r="8" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>359</v>
       </c>
@@ -1913,6 +1912,9 @@
       <c r="O8"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>355</v>
+      </c>
       <c r="B9" t="s">
         <v>272</v>
       </c>
@@ -1930,7 +1932,10 @@
         <v>231</v>
       </c>
     </row>
-    <row r="10" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>359</v>
+      </c>
       <c r="B10" t="s">
         <v>273</v>
       </c>
@@ -1947,7 +1952,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="11" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>384</v>
       </c>
@@ -1972,6 +1977,9 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>355</v>
+      </c>
       <c r="B12" t="s">
         <v>283</v>
       </c>
@@ -1989,8 +1997,10 @@
         <v>231</v>
       </c>
     </row>
-    <row r="13" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
+    <row r="13" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>359</v>
+      </c>
       <c r="B13" t="s">
         <v>284</v>
       </c>
@@ -2017,6 +2027,9 @@
       <c r="O13"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>355</v>
+      </c>
       <c r="B14" t="s">
         <v>246</v>
       </c>
@@ -2038,7 +2051,10 @@
         <v>adminShowUsers.php</v>
       </c>
     </row>
-    <row r="15" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>359</v>
+      </c>
       <c r="B15" t="s">
         <v>247</v>
       </c>
@@ -2058,7 +2074,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="16" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>370</v>
       </c>
@@ -2099,7 +2115,7 @@
       </c>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>359</v>
       </c>
@@ -2119,7 +2135,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="19" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>384</v>
       </c>
@@ -2140,7 +2156,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="20" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>384</v>
       </c>
@@ -2157,7 +2173,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="21" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>384</v>
       </c>
@@ -2178,7 +2194,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="22" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>370</v>
       </c>
@@ -2201,7 +2217,7 @@
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
     </row>
-    <row r="23" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>370</v>
       </c>
@@ -2224,7 +2240,7 @@
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
     </row>
-    <row r="24" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>370</v>
       </c>
@@ -2291,7 +2307,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="26" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>359</v>
       </c>
@@ -2366,7 +2382,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="28" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>359</v>
       </c>
@@ -2401,7 +2417,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="29" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>355</v>
       </c>
@@ -2427,7 +2443,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="30" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>370</v>
       </c>
@@ -2447,7 +2463,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="31" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>370</v>
       </c>
@@ -2467,7 +2483,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="32" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>370</v>
       </c>
@@ -2496,7 +2512,7 @@
       <c r="N32"/>
       <c r="O32"/>
     </row>
-    <row r="33" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>370</v>
       </c>
@@ -2516,7 +2532,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="34" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>385</v>
       </c>
@@ -2549,7 +2565,7 @@
       </c>
       <c r="O34"/>
     </row>
-    <row r="35" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>363</v>
       </c>
@@ -2582,7 +2598,7 @@
       </c>
       <c r="O35"/>
     </row>
-    <row r="36" spans="1:15" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>384</v>
       </c>
@@ -2618,7 +2634,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="37" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>386</v>
       </c>
@@ -2675,7 +2691,7 @@
       <c r="N38"/>
       <c r="O38"/>
     </row>
-    <row r="39" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>363</v>
       </c>
@@ -2723,7 +2739,7 @@
       <c r="N40"/>
       <c r="O40"/>
     </row>
-    <row r="41" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>359</v>
       </c>
@@ -2743,7 +2759,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="42" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>370</v>
       </c>
@@ -2772,7 +2788,7 @@
       <c r="N42"/>
       <c r="O42"/>
     </row>
-    <row r="43" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>370</v>
       </c>
@@ -2801,7 +2817,7 @@
       <c r="N43"/>
       <c r="O43"/>
     </row>
-    <row r="44" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>370</v>
       </c>
@@ -2830,7 +2846,7 @@
       <c r="N44"/>
       <c r="O44"/>
     </row>
-    <row r="45" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>370</v>
       </c>
@@ -2859,7 +2875,7 @@
       <c r="N45"/>
       <c r="O45"/>
     </row>
-    <row r="46" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>369</v>
       </c>
@@ -2888,7 +2904,7 @@
       <c r="N46"/>
       <c r="O46"/>
     </row>
-    <row r="47" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>384</v>
       </c>
@@ -2915,7 +2931,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="48" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>384</v>
       </c>
@@ -2941,7 +2957,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="49" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>384</v>
       </c>
@@ -2968,7 +2984,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="50" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>384</v>
       </c>
@@ -3002,7 +3018,7 @@
       </c>
       <c r="O50"/>
     </row>
-    <row r="51" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>384</v>
       </c>
@@ -3029,7 +3045,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="52" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>384</v>
       </c>
@@ -3063,7 +3079,7 @@
       </c>
       <c r="O52"/>
     </row>
-    <row r="53" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>384</v>
       </c>
@@ -3104,7 +3120,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="55" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>370</v>
       </c>
@@ -3117,7 +3133,7 @@
       <c r="G55" s="1"/>
       <c r="I55" s="1"/>
     </row>
-    <row r="56" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>370</v>
       </c>
@@ -3130,7 +3146,7 @@
       <c r="G56" s="1"/>
       <c r="I56" s="1"/>
     </row>
-    <row r="57" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>370</v>
       </c>
@@ -3143,7 +3159,7 @@
       <c r="G57" s="1"/>
       <c r="I57" s="1"/>
     </row>
-    <row r="58" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>370</v>
       </c>
@@ -3156,7 +3172,7 @@
       <c r="G58" s="1"/>
       <c r="I58" s="1"/>
     </row>
-    <row r="59" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>363</v>
       </c>
@@ -3168,7 +3184,7 @@
       </c>
       <c r="G59" s="1"/>
     </row>
-    <row r="60" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>384</v>
       </c>
@@ -3199,7 +3215,7 @@
       <c r="N60" s="1"/>
       <c r="O60" s="1"/>
     </row>
-    <row r="61" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>370</v>
       </c>
@@ -3226,7 +3242,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="62" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>370</v>
       </c>
@@ -3259,7 +3275,7 @@
       </c>
       <c r="O62"/>
     </row>
-    <row r="63" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>370</v>
       </c>
@@ -3286,7 +3302,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="64" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>370</v>
       </c>
@@ -3320,7 +3336,7 @@
       </c>
       <c r="O64"/>
     </row>
-    <row r="65" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>370</v>
       </c>
@@ -3347,7 +3363,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="66" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>370</v>
       </c>
@@ -3381,7 +3397,7 @@
       </c>
       <c r="O66"/>
     </row>
-    <row r="67" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>355</v>
       </c>
@@ -3407,7 +3423,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="68" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>366</v>
       </c>
@@ -3427,7 +3443,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="69" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>363</v>
       </c>
@@ -3453,7 +3469,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="70" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>363</v>
       </c>
@@ -3526,7 +3542,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="72" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>359</v>
       </c>
@@ -3561,7 +3577,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="73" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>384</v>
       </c>
@@ -3603,7 +3619,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="74" spans="1:15" s="1" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>384</v>
       </c>
@@ -3645,7 +3661,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="75" spans="1:15" s="1" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
         <v>384</v>
       </c>
@@ -3715,7 +3731,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="77" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
         <v>359</v>
       </c>
@@ -3792,7 +3808,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="79" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
         <v>359</v>
       </c>
@@ -3827,7 +3843,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="80" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>384</v>
       </c>
@@ -3869,7 +3885,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="81" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>384</v>
       </c>
@@ -3904,7 +3920,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="82" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
         <v>384</v>
       </c>
@@ -3985,7 +4001,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="84" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
         <v>359</v>
       </c>
@@ -4014,7 +4030,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="85" spans="1:15" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
         <v>389</v>
       </c>
@@ -4058,7 +4074,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="86" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
         <v>391</v>
       </c>
@@ -4093,7 +4109,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="87" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
         <v>389</v>
       </c>
@@ -4114,7 +4130,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="88" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
         <v>391</v>
       </c>
@@ -4134,7 +4150,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="89" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
         <v>389</v>
       </c>
@@ -4155,7 +4171,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="90" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
         <v>389</v>
       </c>
@@ -4183,6 +4199,9 @@
       </c>
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A91" s="4" t="s">
+        <v>389</v>
+      </c>
       <c r="B91" t="s">
         <v>343</v>
       </c>
@@ -4200,7 +4219,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="92" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
         <v>391</v>
       </c>
@@ -4226,7 +4245,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="93" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
         <v>363</v>
       </c>
@@ -4262,7 +4281,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="94" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
         <v>384</v>
       </c>
@@ -4293,7 +4312,7 @@
       <c r="N94" s="1"/>
       <c r="O94" s="1"/>
     </row>
-    <row r="95" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
         <v>370</v>
       </c>
@@ -4327,7 +4346,7 @@
       </c>
       <c r="O95" s="1"/>
     </row>
-    <row r="96" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
         <v>370</v>
       </c>
@@ -4360,7 +4379,7 @@
       </c>
       <c r="O96" s="1"/>
     </row>
-    <row r="97" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
         <v>370</v>
       </c>
@@ -4394,7 +4413,7 @@
       </c>
       <c r="O97" s="1"/>
     </row>
-    <row r="98" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
         <v>370</v>
       </c>
@@ -4428,7 +4447,7 @@
       </c>
       <c r="O98" s="1"/>
     </row>
-    <row r="99" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
         <v>370</v>
       </c>
@@ -4462,7 +4481,7 @@
       </c>
       <c r="O99" s="1"/>
     </row>
-    <row r="100" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
         <v>370</v>
       </c>
@@ -4486,7 +4505,7 @@
         <v>staff.php</v>
       </c>
     </row>
-    <row r="101" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
         <v>370</v>
       </c>
@@ -4509,7 +4528,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="102" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
         <v>370</v>
       </c>
@@ -4533,7 +4552,7 @@
         <v>staff_get.php</v>
       </c>
     </row>
-    <row r="103" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
         <v>370</v>
       </c>
@@ -4557,7 +4576,7 @@
         <v>staff_patch.php</v>
       </c>
     </row>
-    <row r="104" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
         <v>370</v>
       </c>
@@ -4606,7 +4625,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="106" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
         <v>359</v>
       </c>
@@ -4629,7 +4648,10 @@
         <v>271</v>
       </c>
     </row>
-    <row r="107" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A107" s="4" t="s">
+        <v>359</v>
+      </c>
       <c r="B107" t="s">
         <v>323</v>
       </c>
@@ -4646,7 +4668,10 @@
         <v>222</v>
       </c>
     </row>
-    <row r="108" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A108" s="4" t="s">
+        <v>359</v>
+      </c>
       <c r="B108" t="s">
         <v>334</v>
       </c>
@@ -4663,7 +4688,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="109" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
         <v>386</v>
       </c>
@@ -4697,7 +4722,7 @@
       </c>
       <c r="O109" s="1"/>
     </row>
-    <row r="110" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
         <v>390</v>
       </c>
@@ -4717,7 +4742,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="111" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
         <v>370</v>
       </c>
@@ -4740,7 +4765,7 @@
       <c r="N111" s="1"/>
       <c r="O111" s="1"/>
     </row>
-    <row r="112" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
         <v>370</v>
       </c>
@@ -4763,7 +4788,7 @@
       <c r="N112" s="1"/>
       <c r="O112" s="1"/>
     </row>
-    <row r="113" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
         <v>370</v>
       </c>
@@ -4786,7 +4811,7 @@
       <c r="N113" s="1"/>
       <c r="O113" s="1"/>
     </row>
-    <row r="114" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
         <v>370</v>
       </c>
@@ -4809,7 +4834,7 @@
       <c r="N114" s="1"/>
       <c r="O114" s="1"/>
     </row>
-    <row r="115" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
         <v>370</v>
       </c>
@@ -4832,7 +4857,7 @@
       <c r="N115" s="1"/>
       <c r="O115" s="1"/>
     </row>
-    <row r="116" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
         <v>370</v>
       </c>
@@ -4855,7 +4880,7 @@
       <c r="N116" s="1"/>
       <c r="O116" s="1"/>
     </row>
-    <row r="117" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
         <v>363</v>
       </c>
@@ -4881,7 +4906,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="118" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
         <v>355</v>
       </c>
@@ -4926,7 +4951,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="119" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
         <v>359</v>
       </c>
@@ -4955,7 +4980,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="120" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
         <v>355</v>
       </c>
@@ -4986,7 +5011,7 @@
       <c r="N120" s="1"/>
       <c r="O120" s="1"/>
     </row>
-    <row r="121" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A121" s="4" t="s">
         <v>359</v>
       </c>
@@ -5009,7 +5034,7 @@
       <c r="N121" s="1"/>
       <c r="O121" s="1"/>
     </row>
-    <row r="122" spans="1:15" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
         <v>386</v>
       </c>
@@ -5066,7 +5091,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="124" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="s">
         <v>359</v>
       </c>
@@ -5086,7 +5111,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="125" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="s">
         <v>370</v>
       </c>
@@ -5113,7 +5138,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="126" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A126" s="4" t="s">
         <v>370</v>
       </c>
@@ -5139,7 +5164,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="127" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A127" s="4" t="s">
         <v>370</v>
       </c>
@@ -5166,7 +5191,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="128" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A128" s="4" t="s">
         <v>370</v>
       </c>
@@ -5193,7 +5218,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="129" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A129" s="4" t="s">
         <v>370</v>
       </c>
@@ -5264,7 +5289,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="131" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A131" s="4" t="s">
         <v>359</v>
       </c>
@@ -5337,7 +5362,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="133" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A133" s="4" t="s">
         <v>359</v>
       </c>
@@ -5410,7 +5435,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="135" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A135" s="4" t="s">
         <v>359</v>
       </c>
@@ -5482,7 +5507,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="137" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A137" s="4" t="s">
         <v>359</v>
       </c>
@@ -5511,7 +5536,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="138" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A138" s="4" t="s">
         <v>355</v>
       </c>
@@ -5531,7 +5556,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="139" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A139" s="4" t="s">
         <v>359</v>
       </c>
@@ -5553,16 +5578,6 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:O139">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="root"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="2">
-      <filters>
-        <filter val="UI"/>
-      </filters>
-    </filterColumn>
     <sortState ref="A2:O139">
       <sortCondition ref="B1:B139"/>
     </sortState>

</xml_diff>

<commit_message>
Updated file descriptions and fixed uninitialized variable
</commit_message>
<xml_diff>
--- a/tools/web file descriptions.xlsx
+++ b/tools/web file descriptions.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1427" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1461" uniqueCount="448">
   <si>
     <t>addPatient.php</t>
   </si>
@@ -1398,6 +1398,12 @@
   </si>
   <si>
     <t>Logging utilities</t>
+  </si>
+  <si>
+    <t>adminBackup.php</t>
+  </si>
+  <si>
+    <t>System backup interface</t>
   </si>
 </sst>
 </file>
@@ -1758,12 +1764,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:O156"/>
+  <dimension ref="A1:O157"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="615" topLeftCell="A7" activePane="bottomLeft"/>
-      <selection pane="bottomLeft" activeCell="B105" sqref="B105"/>
+      <pane ySplit="615" topLeftCell="A138" activePane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="G157" sqref="G157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1822,7 +1827,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>381</v>
       </c>
@@ -1849,7 +1854,7 @@
       <c r="N2"/>
       <c r="O2"/>
     </row>
-    <row r="3" spans="1:15" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>381</v>
       </c>
@@ -1879,7 +1884,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="4" spans="1:15" s="1" customFormat="1" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>379</v>
       </c>
@@ -1909,7 +1914,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="5" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>381</v>
       </c>
@@ -1945,7 +1950,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="6" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>381</v>
       </c>
@@ -2044,7 +2049,7 @@
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
     </row>
-    <row r="9" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>356</v>
       </c>
@@ -2098,7 +2103,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="11" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>356</v>
       </c>
@@ -2118,7 +2123,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="12" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>379</v>
       </c>
@@ -2165,7 +2170,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="14" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>356</v>
       </c>
@@ -2221,7 +2226,7 @@
         <v>adminShowUsers.php</v>
       </c>
     </row>
-    <row r="16" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>356</v>
       </c>
@@ -2244,7 +2249,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="17" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>367</v>
       </c>
@@ -2288,7 +2293,7 @@
       </c>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>356</v>
       </c>
@@ -2329,7 +2334,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="21" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>379</v>
       </c>
@@ -2367,7 +2372,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="23" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>367</v>
       </c>
@@ -2390,7 +2395,7 @@
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
     </row>
-    <row r="24" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>367</v>
       </c>
@@ -2413,7 +2418,7 @@
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
     </row>
-    <row r="25" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>367</v>
       </c>
@@ -2430,7 +2435,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="26" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>367</v>
       </c>
@@ -2499,7 +2504,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="28" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>356</v>
       </c>
@@ -2576,7 +2581,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="30" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>356</v>
       </c>
@@ -2611,7 +2616,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="31" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>352</v>
       </c>
@@ -2637,7 +2642,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="32" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>367</v>
       </c>
@@ -2657,7 +2662,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="33" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>367</v>
       </c>
@@ -2686,7 +2691,7 @@
       <c r="N33"/>
       <c r="O33"/>
     </row>
-    <row r="34" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>367</v>
       </c>
@@ -2706,7 +2711,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="35" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>367</v>
       </c>
@@ -2735,7 +2740,7 @@
       <c r="N35"/>
       <c r="O35"/>
     </row>
-    <row r="36" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>380</v>
       </c>
@@ -2768,7 +2773,7 @@
       </c>
       <c r="O36"/>
     </row>
-    <row r="37" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>360</v>
       </c>
@@ -2794,7 +2799,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="38" spans="1:15" s="1" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>379</v>
       </c>
@@ -2824,7 +2829,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="39" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>381</v>
       </c>
@@ -2874,7 +2879,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="41" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>360</v>
       </c>
@@ -2926,7 +2931,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="43" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>356</v>
       </c>
@@ -2955,7 +2960,7 @@
       <c r="N43"/>
       <c r="O43"/>
     </row>
-    <row r="44" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>367</v>
       </c>
@@ -2984,7 +2989,7 @@
       <c r="N44"/>
       <c r="O44"/>
     </row>
-    <row r="45" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>367</v>
       </c>
@@ -3013,7 +3018,7 @@
       <c r="N45"/>
       <c r="O45"/>
     </row>
-    <row r="46" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>367</v>
       </c>
@@ -3042,7 +3047,7 @@
       <c r="N46"/>
       <c r="O46"/>
     </row>
-    <row r="47" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>367</v>
       </c>
@@ -3071,7 +3076,7 @@
       <c r="N47"/>
       <c r="O47"/>
     </row>
-    <row r="48" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>366</v>
       </c>
@@ -3091,7 +3096,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="49" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>379</v>
       </c>
@@ -3118,7 +3123,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="50" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>379</v>
       </c>
@@ -3144,7 +3149,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="51" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>379</v>
       </c>
@@ -3178,7 +3183,7 @@
       </c>
       <c r="O51"/>
     </row>
-    <row r="52" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>379</v>
       </c>
@@ -3205,7 +3210,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="53" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>379</v>
       </c>
@@ -3239,7 +3244,7 @@
       </c>
       <c r="O53"/>
     </row>
-    <row r="54" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>379</v>
       </c>
@@ -3266,7 +3271,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="55" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>379</v>
       </c>
@@ -3310,7 +3315,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="57" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>367</v>
       </c>
@@ -3330,7 +3335,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="58" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>367</v>
       </c>
@@ -3350,7 +3355,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="59" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>367</v>
       </c>
@@ -3369,7 +3374,7 @@
       <c r="G59" s="1"/>
       <c r="I59" s="1"/>
     </row>
-    <row r="60" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>367</v>
       </c>
@@ -3388,7 +3393,7 @@
       <c r="G60" s="1"/>
       <c r="I60" s="1"/>
     </row>
-    <row r="61" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>367</v>
       </c>
@@ -3407,7 +3412,7 @@
       <c r="G61" s="1"/>
       <c r="I61" s="1"/>
     </row>
-    <row r="62" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>367</v>
       </c>
@@ -3426,7 +3431,7 @@
       <c r="G62" s="1"/>
       <c r="I62" s="1"/>
     </row>
-    <row r="63" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>360</v>
       </c>
@@ -3452,7 +3457,7 @@
       <c r="N63"/>
       <c r="O63"/>
     </row>
-    <row r="64" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>379</v>
       </c>
@@ -3483,7 +3488,7 @@
       <c r="N64" s="1"/>
       <c r="O64" s="1"/>
     </row>
-    <row r="65" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>367</v>
       </c>
@@ -3517,7 +3522,7 @@
       </c>
       <c r="O65"/>
     </row>
-    <row r="66" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>367</v>
       </c>
@@ -3543,7 +3548,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="67" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>367</v>
       </c>
@@ -3577,7 +3582,7 @@
       </c>
       <c r="O67"/>
     </row>
-    <row r="68" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>367</v>
       </c>
@@ -3604,7 +3609,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="69" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>367</v>
       </c>
@@ -3631,7 +3636,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="70" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>367</v>
       </c>
@@ -3658,7 +3663,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="71" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
         <v>352</v>
       </c>
@@ -3691,7 +3696,7 @@
       <c r="N71"/>
       <c r="O71"/>
     </row>
-    <row r="72" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>363</v>
       </c>
@@ -3720,7 +3725,7 @@
       <c r="N72"/>
       <c r="O72"/>
     </row>
-    <row r="73" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>434</v>
       </c>
@@ -3749,7 +3754,7 @@
       <c r="N73"/>
       <c r="O73"/>
     </row>
-    <row r="74" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>434</v>
       </c>
@@ -3778,7 +3783,7 @@
       <c r="N74"/>
       <c r="O74"/>
     </row>
-    <row r="75" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
         <v>360</v>
       </c>
@@ -3811,7 +3816,7 @@
       </c>
       <c r="O75"/>
     </row>
-    <row r="76" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
         <v>360</v>
       </c>
@@ -3887,7 +3892,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="78" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>356</v>
       </c>
@@ -4006,7 +4011,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="81" spans="1:15" s="1" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>379</v>
       </c>
@@ -4079,7 +4084,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="83" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
         <v>356</v>
       </c>
@@ -4159,7 +4164,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="85" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
         <v>356</v>
       </c>
@@ -4238,7 +4243,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="87" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
         <v>379</v>
       </c>
@@ -4355,7 +4360,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="90" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
         <v>356</v>
       </c>
@@ -4459,7 +4464,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="93" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
         <v>384</v>
       </c>
@@ -4482,7 +4487,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="94" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
         <v>385</v>
       </c>
@@ -4563,7 +4568,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="97" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
         <v>384</v>
       </c>
@@ -4586,7 +4591,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="98" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
         <v>385</v>
       </c>
@@ -4606,7 +4611,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="99" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
         <v>384</v>
       </c>
@@ -4675,7 +4680,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="102" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
         <v>384</v>
       </c>
@@ -4721,7 +4726,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="104" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
         <v>384</v>
       </c>
@@ -4773,7 +4778,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="106" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
         <v>384</v>
       </c>
@@ -4796,7 +4801,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="107" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
         <v>385</v>
       </c>
@@ -4822,7 +4827,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="108" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
         <v>360</v>
       </c>
@@ -4858,7 +4863,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="109" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
         <v>379</v>
       </c>
@@ -4889,7 +4894,7 @@
       <c r="N109" s="1"/>
       <c r="O109" s="1"/>
     </row>
-    <row r="110" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
         <v>367</v>
       </c>
@@ -4923,7 +4928,7 @@
       </c>
       <c r="O110" s="1"/>
     </row>
-    <row r="111" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
         <v>367</v>
       </c>
@@ -4956,7 +4961,7 @@
       </c>
       <c r="O111" s="1"/>
     </row>
-    <row r="112" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
         <v>367</v>
       </c>
@@ -4990,7 +4995,7 @@
       </c>
       <c r="O112" s="1"/>
     </row>
-    <row r="113" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
         <v>367</v>
       </c>
@@ -5024,7 +5029,7 @@
       </c>
       <c r="O113" s="1"/>
     </row>
-    <row r="114" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
         <v>367</v>
       </c>
@@ -5044,7 +5049,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="115" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
         <v>367</v>
       </c>
@@ -5078,7 +5083,7 @@
       </c>
       <c r="O115" s="1"/>
     </row>
-    <row r="116" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
         <v>367</v>
       </c>
@@ -5102,7 +5107,7 @@
         <v>staff.php</v>
       </c>
     </row>
-    <row r="117" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
         <v>367</v>
       </c>
@@ -5125,7 +5130,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="118" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
         <v>367</v>
       </c>
@@ -5145,7 +5150,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="119" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
         <v>367</v>
       </c>
@@ -5169,7 +5174,7 @@
         <v>staff_get.php</v>
       </c>
     </row>
-    <row r="120" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
         <v>367</v>
       </c>
@@ -5193,7 +5198,7 @@
         <v>staff_patch.php</v>
       </c>
     </row>
-    <row r="121" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A121" s="4" t="s">
         <v>367</v>
       </c>
@@ -5244,7 +5249,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="123" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A123" s="4" t="s">
         <v>356</v>
       </c>
@@ -5267,7 +5272,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="124" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="s">
         <v>356</v>
       </c>
@@ -5287,7 +5292,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="125" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="s">
         <v>356</v>
       </c>
@@ -5307,7 +5312,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="126" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A126" s="4" t="s">
         <v>381</v>
       </c>
@@ -5341,7 +5346,7 @@
       </c>
       <c r="O126" s="1"/>
     </row>
-    <row r="127" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A127" s="4" t="s">
         <v>440</v>
       </c>
@@ -5361,7 +5366,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="128" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A128" s="4" t="s">
         <v>367</v>
       </c>
@@ -5388,7 +5393,7 @@
       <c r="N128" s="1"/>
       <c r="O128" s="1"/>
     </row>
-    <row r="129" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A129" s="4" t="s">
         <v>367</v>
       </c>
@@ -5415,7 +5420,7 @@
       <c r="N129" s="1"/>
       <c r="O129" s="1"/>
     </row>
-    <row r="130" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="s">
         <v>367</v>
       </c>
@@ -5442,7 +5447,7 @@
       <c r="N130" s="1"/>
       <c r="O130" s="1"/>
     </row>
-    <row r="131" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A131" s="4" t="s">
         <v>367</v>
       </c>
@@ -5469,7 +5474,7 @@
       <c r="N131" s="1"/>
       <c r="O131" s="1"/>
     </row>
-    <row r="132" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A132" s="4" t="s">
         <v>367</v>
       </c>
@@ -5496,7 +5501,7 @@
       <c r="N132" s="1"/>
       <c r="O132" s="1"/>
     </row>
-    <row r="133" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A133" s="4" t="s">
         <v>367</v>
       </c>
@@ -5523,7 +5528,7 @@
       <c r="N133" s="1"/>
       <c r="O133" s="1"/>
     </row>
-    <row r="134" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A134" s="4" t="s">
         <v>360</v>
       </c>
@@ -5549,7 +5554,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="135" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A135" s="4" t="s">
         <v>352</v>
       </c>
@@ -5594,7 +5599,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="136" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A136" s="4" t="s">
         <v>356</v>
       </c>
@@ -5623,7 +5628,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="137" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A137" s="4" t="s">
         <v>352</v>
       </c>
@@ -5654,7 +5659,7 @@
       <c r="N137" s="1"/>
       <c r="O137" s="1"/>
     </row>
-    <row r="138" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A138" s="4" t="s">
         <v>356</v>
       </c>
@@ -5677,7 +5682,7 @@
       <c r="N138" s="1"/>
       <c r="O138" s="1"/>
     </row>
-    <row r="139" spans="1:15" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A139" s="4" t="s">
         <v>381</v>
       </c>
@@ -5736,7 +5741,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="141" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A141" s="4" t="s">
         <v>356</v>
       </c>
@@ -5756,7 +5761,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="142" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A142" s="4" t="s">
         <v>367</v>
       </c>
@@ -5783,7 +5788,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="143" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A143" s="4" t="s">
         <v>367</v>
       </c>
@@ -5809,7 +5814,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="144" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A144" s="4" t="s">
         <v>367</v>
       </c>
@@ -5836,7 +5841,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="145" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A145" s="4" t="s">
         <v>367</v>
       </c>
@@ -5863,7 +5868,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="146" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A146" s="4" t="s">
         <v>367</v>
       </c>
@@ -5936,7 +5941,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="148" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A148" s="4" t="s">
         <v>356</v>
       </c>
@@ -6011,7 +6016,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="150" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A150" s="4" t="s">
         <v>356</v>
       </c>
@@ -6086,7 +6091,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="152" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A152" s="4" t="s">
         <v>356</v>
       </c>
@@ -6160,7 +6165,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="154" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A154" s="4" t="s">
         <v>356</v>
       </c>
@@ -6189,7 +6194,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="155" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A155" s="4" t="s">
         <v>352</v>
       </c>
@@ -6209,7 +6214,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="156" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A156" s="4" t="s">
         <v>356</v>
       </c>
@@ -6229,13 +6234,28 @@
         <v>222</v>
       </c>
     </row>
+    <row r="157" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A157" s="4" t="s">
+        <v>352</v>
+      </c>
+      <c r="B157" t="s">
+        <v>446</v>
+      </c>
+      <c r="C157" t="s">
+        <v>97</v>
+      </c>
+      <c r="E157" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="F157" t="s">
+        <v>447</v>
+      </c>
+      <c r="G157" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:O156">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="UI"/>
-      </filters>
-    </filterColumn>
     <sortState ref="A2:O156">
       <sortCondition ref="B1:B156"/>
     </sortState>
@@ -6247,9 +6267,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G125"/>
+  <dimension ref="A1:J125"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6257,7 +6279,7 @@
     <col min="6" max="6" width="25.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>280</v>
       </c>
@@ -6266,14 +6288,17 @@
         <v>addComment.php</v>
       </c>
       <c r="F1" t="s">
-        <v>401</v>
+        <v>446</v>
       </c>
       <c r="G1" t="str">
         <f>VLOOKUP(F1,Current!B$2:B$193,1,FALSE)</f>
-        <v>adminHelpAddEdit.php</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>adminBackup.php</v>
+      </c>
+      <c r="J1" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -6282,14 +6307,17 @@
         <v>addPatient.php</v>
       </c>
       <c r="F2" t="s">
-        <v>244</v>
+        <v>401</v>
       </c>
       <c r="G2" t="str">
         <f>VLOOKUP(F2,Current!B$2:B$193,1,FALSE)</f>
-        <v>adminHome.php</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>adminHelpAddEdit.php</v>
+      </c>
+      <c r="J2" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -6298,14 +6326,17 @@
         <v>addPatientImage.php</v>
       </c>
       <c r="F3" t="s">
-        <v>272</v>
+        <v>244</v>
       </c>
       <c r="G3" t="str">
         <f>VLOOKUP(F3,Current!B$2:B$193,1,FALSE)</f>
-        <v>adminLogViewer.php</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>adminHome.php</v>
+      </c>
+      <c r="J3" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -6314,14 +6345,17 @@
         <v>addPatientVisit.php</v>
       </c>
       <c r="F4" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="G4" t="str">
         <f>VLOOKUP(F4,Current!B$2:B$193,1,FALSE)</f>
-        <v>adminShowComments.php</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>adminLogViewer.php</v>
+      </c>
+      <c r="J4" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>243</v>
       </c>
@@ -6330,14 +6364,17 @@
         <v>addStaff.php</v>
       </c>
       <c r="F5" t="s">
-        <v>246</v>
+        <v>281</v>
       </c>
       <c r="G5" t="str">
         <f>VLOOKUP(F5,Current!B$2:B$193,1,FALSE)</f>
-        <v>adminShowUsers.php</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>adminShowComments.php</v>
+      </c>
+      <c r="J5" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>244</v>
       </c>
@@ -6346,14 +6383,17 @@
         <v>adminHome.php</v>
       </c>
       <c r="F6" t="s">
-        <v>353</v>
+        <v>246</v>
       </c>
       <c r="G6" t="str">
         <f>VLOOKUP(F6,Current!B$2:B$193,1,FALSE)</f>
-        <v>appMenu.php</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>adminShowUsers.php</v>
+      </c>
+      <c r="J6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>245</v>
       </c>
@@ -6362,14 +6402,17 @@
         <v>adminHomeText.php</v>
       </c>
       <c r="F7" t="s">
-        <v>65</v>
+        <v>353</v>
       </c>
       <c r="G7" t="str">
         <f>VLOOKUP(F7,Current!B$2:B$193,1,FALSE)</f>
-        <v>clinicDash.php</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>appMenu.php</v>
+      </c>
+      <c r="J7" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>272</v>
       </c>
@@ -6378,14 +6421,17 @@
         <v>adminLogViewer.php</v>
       </c>
       <c r="F8" t="s">
-        <v>189</v>
+        <v>65</v>
       </c>
       <c r="G8" t="str">
         <f>VLOOKUP(F8,Current!B$2:B$193,1,FALSE)</f>
-        <v>clinicLogin.php</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>clinicDash.php</v>
+      </c>
+      <c r="J8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>273</v>
       </c>
@@ -6394,14 +6440,17 @@
         <v>adminLogViewerText.php</v>
       </c>
       <c r="F9" t="s">
-        <v>304</v>
+        <v>189</v>
       </c>
       <c r="G9" t="str">
         <f>VLOOKUP(F9,Current!B$2:B$193,1,FALSE)</f>
-        <v>code39.php</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>clinicLogin.php</v>
+      </c>
+      <c r="J9" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>281</v>
       </c>
@@ -6410,14 +6459,17 @@
         <v>adminShowComments.php</v>
       </c>
       <c r="F10" t="s">
-        <v>287</v>
+        <v>304</v>
       </c>
       <c r="G10" t="str">
         <f>VLOOKUP(F10,Current!B$2:B$193,1,FALSE)</f>
-        <v>helpHome.php</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>code39.php</v>
+      </c>
+      <c r="J10" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>282</v>
       </c>
@@ -6426,14 +6478,17 @@
         <v>adminShowCommentsText.php</v>
       </c>
       <c r="F11" t="s">
-        <v>354</v>
+        <v>287</v>
       </c>
       <c r="G11" t="str">
         <f>VLOOKUP(F11,Current!B$2:B$193,1,FALSE)</f>
-        <v>index.php</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>helpHome.php</v>
+      </c>
+      <c r="J11" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>246</v>
       </c>
@@ -6442,14 +6497,17 @@
         <v>adminShowUsers.php</v>
       </c>
       <c r="F12" t="s">
-        <v>19</v>
+        <v>354</v>
       </c>
       <c r="G12" t="str">
         <f>VLOOKUP(F12,Current!B$2:B$193,1,FALSE)</f>
-        <v>phpinfo.php</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>index.php</v>
+      </c>
+      <c r="J12" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>247</v>
       </c>
@@ -6458,14 +6516,17 @@
         <v>adminShowUsersText.php</v>
       </c>
       <c r="F13" t="s">
-        <v>69</v>
+        <v>19</v>
       </c>
       <c r="G13" t="str">
         <f>VLOOKUP(F13,Current!B$2:B$193,1,FALSE)</f>
-        <v>ptAddEdit.php</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>phpinfo.php</v>
+      </c>
+      <c r="J13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -6474,14 +6535,17 @@
         <v>api_common.php</v>
       </c>
       <c r="F14" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="G14" t="str">
         <f>VLOOKUP(F14,Current!B$2:B$193,1,FALSE)</f>
-        <v>ptInfo.php</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>ptAddEdit.php</v>
+      </c>
+      <c r="J14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>274</v>
       </c>
@@ -6490,14 +6554,17 @@
         <v>appMenuText.php</v>
       </c>
       <c r="F15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G15" t="str">
         <f>VLOOKUP(F15,Current!B$2:B$193,1,FALSE)</f>
-        <v>ptResults.php</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>ptInfo.php</v>
+      </c>
+      <c r="J15" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>347</v>
       </c>
@@ -6506,14 +6573,17 @@
         <v>#N/A</v>
       </c>
       <c r="F16" t="s">
-        <v>355</v>
+        <v>90</v>
       </c>
       <c r="G16" t="str">
         <f>VLOOKUP(F16,Current!B$2:B$193,1,FALSE)</f>
-        <v>reportHome.php</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>ptResults.php</v>
+      </c>
+      <c r="J16" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>321</v>
       </c>
@@ -6522,14 +6592,17 @@
         <v>#N/A</v>
       </c>
       <c r="F17" t="s">
-        <v>249</v>
+        <v>355</v>
       </c>
       <c r="G17" t="str">
         <f>VLOOKUP(F17,Current!B$2:B$193,1,FALSE)</f>
-        <v>staffAddEdit.php</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>reportHome.php</v>
+      </c>
+      <c r="J17" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>329</v>
       </c>
@@ -6538,14 +6611,17 @@
         <v>ataEntryText.php</v>
       </c>
       <c r="F18" t="s">
-        <v>320</v>
+        <v>249</v>
       </c>
       <c r="G18" t="str">
         <f>VLOOKUP(F18,Current!B$2:B$193,1,FALSE)</f>
-        <v>staffUiStrings.php</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>staffAddEdit.php</v>
+      </c>
+      <c r="J18" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>330</v>
       </c>
@@ -6554,14 +6630,17 @@
         <v>ataVisitEdit.php</v>
       </c>
       <c r="F19" t="s">
-        <v>96</v>
+        <v>320</v>
       </c>
       <c r="G19" t="str">
         <f>VLOOKUP(F19,Current!B$2:B$193,1,FALSE)</f>
-        <v>uiErrorMessage.php</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>staffUiStrings.php</v>
+      </c>
+      <c r="J19" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>65</v>
       </c>
@@ -6570,14 +6649,17 @@
         <v>clinicDash.php</v>
       </c>
       <c r="F20" t="s">
-        <v>233</v>
+        <v>96</v>
       </c>
       <c r="G20" t="str">
         <f>VLOOKUP(F20,Current!B$2:B$193,1,FALSE)</f>
-        <v>uiSessionInfo.php</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>uiErrorMessage.php</v>
+      </c>
+      <c r="J20" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>66</v>
       </c>
@@ -6586,14 +6668,17 @@
         <v>clinicDashText.php</v>
       </c>
       <c r="F21" t="s">
-        <v>289</v>
+        <v>233</v>
       </c>
       <c r="G21" t="str">
         <f>VLOOKUP(F21,Current!B$2:B$193,1,FALSE)</f>
-        <v>userComment.php</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <v>uiSessionInfo.php</v>
+      </c>
+      <c r="J21" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>189</v>
       </c>
@@ -6602,14 +6687,17 @@
         <v>clinicLogin.php</v>
       </c>
       <c r="F22" t="s">
-        <v>92</v>
+        <v>289</v>
       </c>
       <c r="G22" t="str">
         <f>VLOOKUP(F22,Current!B$2:B$193,1,FALSE)</f>
-        <v>visitClose.php</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>userComment.php</v>
+      </c>
+      <c r="J22" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>190</v>
       </c>
@@ -6618,14 +6706,17 @@
         <v>clinicLoginText.php</v>
       </c>
       <c r="F23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G23" t="str">
         <f>VLOOKUP(F23,Current!B$2:B$193,1,FALSE)</f>
-        <v>visitEdit.php</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+        <v>visitClose.php</v>
+      </c>
+      <c r="J23" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>304</v>
       </c>
@@ -6634,14 +6725,17 @@
         <v>code39.php</v>
       </c>
       <c r="F24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G24" t="str">
         <f>VLOOKUP(F24,Current!B$2:B$193,1,FALSE)</f>
-        <v>visitInfo.php</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>visitEdit.php</v>
+      </c>
+      <c r="J24" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>283</v>
       </c>
@@ -6650,14 +6744,17 @@
         <v>comment.php</v>
       </c>
       <c r="F25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G25" t="str">
         <f>VLOOKUP(F25,Current!B$2:B$193,1,FALSE)</f>
-        <v>visitOpen.php</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>visitInfo.php</v>
+      </c>
+      <c r="J25" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>284</v>
       </c>
@@ -6666,14 +6763,17 @@
         <v>comment_common.php</v>
       </c>
       <c r="F26" t="s">
-        <v>332</v>
+        <v>95</v>
       </c>
       <c r="G26" t="str">
         <f>VLOOKUP(F26,Current!B$2:B$193,1,FALSE)</f>
-        <v>visitUiStrings.php</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+        <v>visitOpen.php</v>
+      </c>
+      <c r="J26" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>285</v>
       </c>
@@ -6681,8 +6781,18 @@
         <f>VLOOKUP(A27,Current!B$2:B$143,1,FALSE)</f>
         <v>comment_get.php</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F27" t="s">
+        <v>332</v>
+      </c>
+      <c r="G27" t="str">
+        <f>VLOOKUP(F27,Current!B$2:B$193,1,FALSE)</f>
+        <v>visitUiStrings.php</v>
+      </c>
+      <c r="J27" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>286</v>
       </c>
@@ -6691,7 +6801,7 @@
         <v>comment_post.php</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -6699,15 +6809,12 @@
         <f>VLOOKUP(A29,Current!B$2:B$143,1,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F29" t="s">
-        <v>406</v>
-      </c>
       <c r="G29" t="str">
-        <f>VLOOKUP(F29,Current!B$2:B$193,1,FALSE)</f>
+        <f>VLOOKUP(F30,Current!B$2:B$193,1,FALSE)</f>
         <v>rptDailyLogHome.php</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>5</v>
       </c>
@@ -6716,14 +6823,14 @@
         <v>dbPass.php</v>
       </c>
       <c r="F30" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="G30" t="str">
-        <f>VLOOKUP(F30,Current!B$2:B$193,1,FALSE)</f>
+        <f>VLOOKUP(F31,Current!B$2:B$193,1,FALSE)</f>
         <v>rptDailyLogMenu.php</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>6</v>
       </c>
@@ -6732,14 +6839,14 @@
         <v>#N/A</v>
       </c>
       <c r="F31" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="G31" t="str">
-        <f>VLOOKUP(F31,Current!B$2:B$193,1,FALSE)</f>
+        <f>VLOOKUP(F32,Current!B$2:B$193,1,FALSE)</f>
         <v>rptDailyPmtHome.php</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>119</v>
       </c>
@@ -6748,10 +6855,10 @@
         <v>deletePatientImage.php</v>
       </c>
       <c r="F32" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="G32" t="str">
-        <f>VLOOKUP(F32,Current!B$2:B$193,1,FALSE)</f>
+        <f>VLOOKUP(F33,Current!B$2:B$193,1,FALSE)</f>
         <v>rptDailyPmtMenu.php</v>
       </c>
     </row>
@@ -6764,10 +6871,10 @@
         <v>endUiSession.php</v>
       </c>
       <c r="F33" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="G33" t="str">
-        <f>VLOOKUP(F33,Current!B$2:B$193,1,FALSE)</f>
+        <f>VLOOKUP(F34,Current!B$2:B$193,1,FALSE)</f>
         <v>rptGroups.php</v>
       </c>
     </row>
@@ -6780,10 +6887,10 @@
         <v>headTag.php</v>
       </c>
       <c r="F34" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G34" t="str">
-        <f>VLOOKUP(F34,Current!B$2:B$193,1,FALSE)</f>
+        <f>VLOOKUP(F35,Current!B$2:B$193,1,FALSE)</f>
         <v>rptMonthlyPmtHome.php</v>
       </c>
     </row>
@@ -6796,10 +6903,10 @@
         <v>helpHome.php</v>
       </c>
       <c r="F35" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G35" t="str">
-        <f>VLOOKUP(F35,Current!B$2:B$193,1,FALSE)</f>
+        <f>VLOOKUP(F36,Current!B$2:B$193,1,FALSE)</f>
         <v>rptMonthlyPmtMenu.php</v>
       </c>
     </row>
@@ -6812,10 +6919,10 @@
         <v>helpHomeText.php</v>
       </c>
       <c r="F36" t="s">
-        <v>400</v>
+        <v>412</v>
       </c>
       <c r="G36" t="str">
-        <f>VLOOKUP(F36,Current!B$2:B$193,1,FALSE)</f>
+        <f>VLOOKUP(F37,Current!B$2:B$193,1,FALSE)</f>
         <v>rptMonthlyPosSummHome.php</v>
       </c>
     </row>
@@ -6828,10 +6935,10 @@
         <v>icd.php</v>
       </c>
       <c r="F37" t="s">
-        <v>413</v>
+        <v>400</v>
       </c>
       <c r="G37" t="str">
-        <f>VLOOKUP(F37,Current!B$2:B$193,1,FALSE)</f>
+        <f>VLOOKUP(F38,Current!B$2:B$193,1,FALSE)</f>
         <v>rptMonthlyPosSummMenu.php</v>
       </c>
     </row>
@@ -6844,10 +6951,10 @@
         <v>icd_common.php</v>
       </c>
       <c r="F38" t="s">
-        <v>399</v>
+        <v>413</v>
       </c>
       <c r="G38" t="str">
-        <f>VLOOKUP(F38,Current!B$2:B$193,1,FALSE)</f>
+        <f>VLOOKUP(F39,Current!B$2:B$193,1,FALSE)</f>
         <v>rptMonthlyPtSummHome.php</v>
       </c>
     </row>
@@ -6860,10 +6967,10 @@
         <v>icd_get.php</v>
       </c>
       <c r="F39" t="s">
-        <v>414</v>
+        <v>399</v>
       </c>
       <c r="G39" t="str">
-        <f>VLOOKUP(F39,Current!B$2:B$193,1,FALSE)</f>
+        <f>VLOOKUP(F40,Current!B$2:B$193,1,FALSE)</f>
         <v>rptMonthlyPtSummMenu.php</v>
       </c>
     </row>
@@ -6875,6 +6982,9 @@
         <f>VLOOKUP(A40,Current!B$2:B$143,1,FALSE)</f>
         <v>icd_patch.php</v>
       </c>
+      <c r="F40" t="s">
+        <v>414</v>
+      </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
@@ -6884,11 +6994,8 @@
         <f>VLOOKUP(A41,Current!B$2:B$143,1,FALSE)</f>
         <v>image.php</v>
       </c>
-      <c r="F41" t="s">
-        <v>3</v>
-      </c>
       <c r="G41" t="str">
-        <f>VLOOKUP(F41,Current!B$2:B$193,1,FALSE)</f>
+        <f>VLOOKUP(F42,Current!B$2:B$193,1,FALSE)</f>
         <v>api_common.php</v>
       </c>
     </row>
@@ -6901,10 +7008,10 @@
         <v>image_common.php</v>
       </c>
       <c r="F42" t="s">
-        <v>368</v>
+        <v>3</v>
       </c>
       <c r="G42" t="str">
-        <f>VLOOKUP(F42,Current!B$2:B$193,1,FALSE)</f>
+        <f>VLOOKUP(F43,Current!B$2:B$193,1,FALSE)</f>
         <v>clinic.php</v>
       </c>
     </row>
@@ -6917,10 +7024,10 @@
         <v>image_delete.php</v>
       </c>
       <c r="F43" t="s">
-        <v>417</v>
+        <v>368</v>
       </c>
       <c r="G43" t="str">
-        <f>VLOOKUP(F43,Current!B$2:B$193,1,FALSE)</f>
+        <f>VLOOKUP(F44,Current!B$2:B$193,1,FALSE)</f>
         <v>clinic_common.php</v>
       </c>
     </row>
@@ -6933,10 +7040,10 @@
         <v>image_get.php</v>
       </c>
       <c r="F44" t="s">
-        <v>370</v>
+        <v>417</v>
       </c>
       <c r="G44" t="str">
-        <f>VLOOKUP(F44,Current!B$2:B$193,1,FALSE)</f>
+        <f>VLOOKUP(F45,Current!B$2:B$193,1,FALSE)</f>
         <v>clinic_get.php</v>
       </c>
     </row>
@@ -6949,10 +7056,10 @@
         <v>image_patch.php</v>
       </c>
       <c r="F45" t="s">
-        <v>283</v>
+        <v>370</v>
       </c>
       <c r="G45" t="str">
-        <f>VLOOKUP(F45,Current!B$2:B$193,1,FALSE)</f>
+        <f>VLOOKUP(F46,Current!B$2:B$193,1,FALSE)</f>
         <v>comment.php</v>
       </c>
     </row>
@@ -6965,10 +7072,10 @@
         <v>image_post.php</v>
       </c>
       <c r="F46" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G46" t="str">
-        <f>VLOOKUP(F46,Current!B$2:B$193,1,FALSE)</f>
+        <f>VLOOKUP(F47,Current!B$2:B$193,1,FALSE)</f>
         <v>comment_common.php</v>
       </c>
     </row>
@@ -6981,10 +7088,10 @@
         <v>image_put.php</v>
       </c>
       <c r="F47" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G47" t="str">
-        <f>VLOOKUP(F47,Current!B$2:B$193,1,FALSE)</f>
+        <f>VLOOKUP(F48,Current!B$2:B$193,1,FALSE)</f>
         <v>comment_get.php</v>
       </c>
     </row>
@@ -6997,10 +7104,10 @@
         <v>pass.php</v>
       </c>
       <c r="F48" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G48" t="str">
-        <f>VLOOKUP(F48,Current!B$2:B$193,1,FALSE)</f>
+        <f>VLOOKUP(F49,Current!B$2:B$193,1,FALSE)</f>
         <v>comment_post.php</v>
       </c>
     </row>
@@ -7013,10 +7120,10 @@
         <v>patient.php</v>
       </c>
       <c r="F49" t="s">
-        <v>316</v>
+        <v>286</v>
       </c>
       <c r="G49" t="str">
-        <f>VLOOKUP(F49,Current!B$2:B$193,1,FALSE)</f>
+        <f>VLOOKUP(F50,Current!B$2:B$193,1,FALSE)</f>
         <v>icd.php</v>
       </c>
     </row>
@@ -7029,10 +7136,10 @@
         <v>patient_common.php</v>
       </c>
       <c r="F50" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G50" t="str">
-        <f>VLOOKUP(F50,Current!B$2:B$193,1,FALSE)</f>
+        <f>VLOOKUP(F51,Current!B$2:B$193,1,FALSE)</f>
         <v>icd_common.php</v>
       </c>
     </row>
@@ -7045,10 +7152,10 @@
         <v>patient_delete.php</v>
       </c>
       <c r="F51" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="G51" t="str">
-        <f>VLOOKUP(F51,Current!B$2:B$193,1,FALSE)</f>
+        <f>VLOOKUP(F52,Current!B$2:B$193,1,FALSE)</f>
         <v>icd_get.php</v>
       </c>
     </row>
@@ -7061,10 +7168,10 @@
         <v>patient_get.php</v>
       </c>
       <c r="F52" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="G52" t="str">
-        <f>VLOOKUP(F52,Current!B$2:B$193,1,FALSE)</f>
+        <f>VLOOKUP(F53,Current!B$2:B$193,1,FALSE)</f>
         <v>icd_patch.php</v>
       </c>
     </row>
@@ -7077,10 +7184,10 @@
         <v>patient_patch.php</v>
       </c>
       <c r="F53" t="s">
-        <v>418</v>
+        <v>319</v>
       </c>
       <c r="G53" t="str">
-        <f>VLOOKUP(F53,Current!B$2:B$193,1,FALSE)</f>
+        <f>VLOOKUP(F54,Current!B$2:B$193,1,FALSE)</f>
         <v>locImage.php</v>
       </c>
     </row>
@@ -7093,10 +7200,10 @@
         <v>patient_post.php</v>
       </c>
       <c r="F54" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G54" t="str">
-        <f>VLOOKUP(F54,Current!B$2:B$193,1,FALSE)</f>
+        <f>VLOOKUP(F55,Current!B$2:B$193,1,FALSE)</f>
         <v>locImage_get.php</v>
       </c>
     </row>
@@ -7109,10 +7216,10 @@
         <v>phpinfo.php</v>
       </c>
       <c r="F55" t="s">
-        <v>371</v>
+        <v>419</v>
       </c>
       <c r="G55" t="str">
-        <f>VLOOKUP(F55,Current!B$2:B$193,1,FALSE)</f>
+        <f>VLOOKUP(F56,Current!B$2:B$193,1,FALSE)</f>
         <v>log.php</v>
       </c>
     </row>
@@ -7125,10 +7232,10 @@
         <v>profile.php</v>
       </c>
       <c r="F56" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="G56" t="str">
-        <f>VLOOKUP(F56,Current!B$2:B$193,1,FALSE)</f>
+        <f>VLOOKUP(F57,Current!B$2:B$193,1,FALSE)</f>
         <v>log_common.php</v>
       </c>
     </row>
@@ -7141,10 +7248,10 @@
         <v>ptAddEdit.php</v>
       </c>
       <c r="F57" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G57" t="str">
-        <f>VLOOKUP(F57,Current!B$2:B$193,1,FALSE)</f>
+        <f>VLOOKUP(F58,Current!B$2:B$193,1,FALSE)</f>
         <v>log_get.php</v>
       </c>
     </row>
@@ -7157,10 +7264,10 @@
         <v>ptAddEditText.php</v>
       </c>
       <c r="F58" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G58" t="str">
-        <f>VLOOKUP(F58,Current!B$2:B$193,1,FALSE)</f>
+        <f>VLOOKUP(F59,Current!B$2:B$193,1,FALSE)</f>
         <v>log_post.php</v>
       </c>
     </row>
@@ -7173,10 +7280,10 @@
         <v>ptImageDeleteConfirm.php</v>
       </c>
       <c r="F59" t="s">
-        <v>13</v>
+        <v>374</v>
       </c>
       <c r="G59" t="str">
-        <f>VLOOKUP(F59,Current!B$2:B$193,1,FALSE)</f>
+        <f>VLOOKUP(F60,Current!B$2:B$193,1,FALSE)</f>
         <v>patient.php</v>
       </c>
     </row>
@@ -7189,10 +7296,10 @@
         <v>ptImageEdit.php</v>
       </c>
       <c r="F60" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G60" t="str">
-        <f>VLOOKUP(F60,Current!B$2:B$193,1,FALSE)</f>
+        <f>VLOOKUP(F61,Current!B$2:B$193,1,FALSE)</f>
         <v>patient_common.php</v>
       </c>
     </row>
@@ -7205,10 +7312,10 @@
         <v>ptImageEditText.php</v>
       </c>
       <c r="F61" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G61" t="str">
-        <f>VLOOKUP(F61,Current!B$2:B$193,1,FALSE)</f>
+        <f>VLOOKUP(F62,Current!B$2:B$193,1,FALSE)</f>
         <v>patient_delete.php</v>
       </c>
     </row>
@@ -7221,10 +7328,10 @@
         <v>ptInfo.php</v>
       </c>
       <c r="F62" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G62" t="str">
-        <f>VLOOKUP(F62,Current!B$2:B$193,1,FALSE)</f>
+        <f>VLOOKUP(F63,Current!B$2:B$193,1,FALSE)</f>
         <v>patient_get.php</v>
       </c>
     </row>
@@ -7237,10 +7344,10 @@
         <v>ptInfoText.php</v>
       </c>
       <c r="F63" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G63" t="str">
-        <f>VLOOKUP(F63,Current!B$2:B$193,1,FALSE)</f>
+        <f>VLOOKUP(F64,Current!B$2:B$193,1,FALSE)</f>
         <v>patient_patch.php</v>
       </c>
     </row>
@@ -7253,10 +7360,10 @@
         <v>ptResults.php</v>
       </c>
       <c r="F64" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G64" t="str">
-        <f>VLOOKUP(F64,Current!B$2:B$193,1,FALSE)</f>
+        <f>VLOOKUP(F65,Current!B$2:B$193,1,FALSE)</f>
         <v>patient_post.php</v>
       </c>
     </row>
@@ -7269,10 +7376,10 @@
         <v>ptResultsText.php</v>
       </c>
       <c r="F65" t="s">
-        <v>194</v>
+        <v>18</v>
       </c>
       <c r="G65" t="str">
-        <f>VLOOKUP(F65,Current!B$2:B$193,1,FALSE)</f>
+        <f>VLOOKUP(F66,Current!B$2:B$193,1,FALSE)</f>
         <v>session.php</v>
       </c>
     </row>
@@ -7285,10 +7392,10 @@
         <v>ptSearch.php</v>
       </c>
       <c r="F66" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G66" t="str">
-        <f>VLOOKUP(F66,Current!B$2:B$193,1,FALSE)</f>
+        <f>VLOOKUP(F67,Current!B$2:B$193,1,FALSE)</f>
         <v>session_common.php</v>
       </c>
     </row>
@@ -7301,10 +7408,10 @@
         <v>ptSearchText.php</v>
       </c>
       <c r="F67" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G67" t="str">
-        <f>VLOOKUP(F67,Current!B$2:B$193,1,FALSE)</f>
+        <f>VLOOKUP(F68,Current!B$2:B$193,1,FALSE)</f>
         <v>session_delete.php</v>
       </c>
     </row>
@@ -7317,10 +7424,10 @@
         <v>ptVisitImageView.php</v>
       </c>
       <c r="F68" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G68" t="str">
-        <f>VLOOKUP(F68,Current!B$2:B$193,1,FALSE)</f>
+        <f>VLOOKUP(F69,Current!B$2:B$193,1,FALSE)</f>
         <v>session_get.php</v>
       </c>
     </row>
@@ -7333,10 +7440,10 @@
         <v>rptDailyLog.php</v>
       </c>
       <c r="F69" t="s">
-        <v>420</v>
+        <v>197</v>
       </c>
       <c r="G69" t="str">
-        <f>VLOOKUP(F69,Current!B$2:B$193,1,FALSE)</f>
+        <f>VLOOKUP(F70,Current!B$2:B$193,1,FALSE)</f>
         <v>session_patch.php</v>
       </c>
     </row>
@@ -7349,10 +7456,10 @@
         <v>rptDailyLogText.php</v>
       </c>
       <c r="F70" t="s">
-        <v>198</v>
+        <v>420</v>
       </c>
       <c r="G70" t="str">
-        <f>VLOOKUP(F70,Current!B$2:B$193,1,FALSE)</f>
+        <f>VLOOKUP(F71,Current!B$2:B$193,1,FALSE)</f>
         <v>session_post.php</v>
       </c>
     </row>
@@ -7365,10 +7472,10 @@
         <v>rptDailyPmt.php</v>
       </c>
       <c r="F71" t="s">
-        <v>248</v>
+        <v>198</v>
       </c>
       <c r="G71" t="str">
-        <f>VLOOKUP(F71,Current!B$2:B$193,1,FALSE)</f>
+        <f>VLOOKUP(F72,Current!B$2:B$193,1,FALSE)</f>
         <v>staff.php</v>
       </c>
     </row>
@@ -7381,10 +7488,10 @@
         <v>rptDailyPmtText.php</v>
       </c>
       <c r="F72" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="G72" t="str">
-        <f>VLOOKUP(F72,Current!B$2:B$193,1,FALSE)</f>
+        <f>VLOOKUP(F73,Current!B$2:B$193,1,FALSE)</f>
         <v>staff_common.php</v>
       </c>
     </row>
@@ -7397,10 +7504,10 @@
         <v>#N/A</v>
       </c>
       <c r="F73" t="s">
-        <v>421</v>
+        <v>251</v>
       </c>
       <c r="G73" t="str">
-        <f>VLOOKUP(F73,Current!B$2:B$193,1,FALSE)</f>
+        <f>VLOOKUP(F74,Current!B$2:B$193,1,FALSE)</f>
         <v>staff_delete.php</v>
       </c>
     </row>
@@ -7413,10 +7520,10 @@
         <v>#N/A</v>
       </c>
       <c r="F74" t="s">
-        <v>252</v>
+        <v>421</v>
       </c>
       <c r="G74" t="str">
-        <f>VLOOKUP(F74,Current!B$2:B$193,1,FALSE)</f>
+        <f>VLOOKUP(F75,Current!B$2:B$193,1,FALSE)</f>
         <v>staff_get.php</v>
       </c>
     </row>
@@ -7429,10 +7536,10 @@
         <v>rptMonthlyPmt.php</v>
       </c>
       <c r="F75" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G75" t="str">
-        <f>VLOOKUP(F75,Current!B$2:B$193,1,FALSE)</f>
+        <f>VLOOKUP(F76,Current!B$2:B$193,1,FALSE)</f>
         <v>staff_patch.php</v>
       </c>
     </row>
@@ -7445,10 +7552,10 @@
         <v>#N/A</v>
       </c>
       <c r="F76" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G76" t="str">
-        <f>VLOOKUP(F76,Current!B$2:B$193,1,FALSE)</f>
+        <f>VLOOKUP(F77,Current!B$2:B$193,1,FALSE)</f>
         <v>staff_post.php</v>
       </c>
     </row>
@@ -7461,10 +7568,10 @@
         <v>#N/A</v>
       </c>
       <c r="F77" t="s">
-        <v>375</v>
+        <v>254</v>
       </c>
       <c r="G77" t="str">
-        <f>VLOOKUP(F77,Current!B$2:B$193,1,FALSE)</f>
+        <f>VLOOKUP(F78,Current!B$2:B$193,1,FALSE)</f>
         <v>textmsg.php</v>
       </c>
     </row>
@@ -7477,10 +7584,10 @@
         <v>rptMonthlySummaryText.php</v>
       </c>
       <c r="F78" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="G78" t="str">
-        <f>VLOOKUP(F78,Current!B$2:B$193,1,FALSE)</f>
+        <f>VLOOKUP(F79,Current!B$2:B$193,1,FALSE)</f>
         <v>textmsg_common.php</v>
       </c>
     </row>
@@ -7493,10 +7600,10 @@
         <v>security.php</v>
       </c>
       <c r="F79" t="s">
-        <v>422</v>
+        <v>376</v>
       </c>
       <c r="G79" t="str">
-        <f>VLOOKUP(F79,Current!B$2:B$193,1,FALSE)</f>
+        <f>VLOOKUP(F80,Current!B$2:B$193,1,FALSE)</f>
         <v>textmsg_delete.php</v>
       </c>
     </row>
@@ -7509,10 +7616,10 @@
         <v>securityText.php</v>
       </c>
       <c r="F80" t="s">
-        <v>377</v>
+        <v>422</v>
       </c>
       <c r="G80" t="str">
-        <f>VLOOKUP(F80,Current!B$2:B$193,1,FALSE)</f>
+        <f>VLOOKUP(F81,Current!B$2:B$193,1,FALSE)</f>
         <v>textmsg_get.php</v>
       </c>
     </row>
@@ -7525,10 +7632,10 @@
         <v>session.php</v>
       </c>
       <c r="F81" t="s">
-        <v>423</v>
+        <v>377</v>
       </c>
       <c r="G81" t="str">
-        <f>VLOOKUP(F81,Current!B$2:B$193,1,FALSE)</f>
+        <f>VLOOKUP(F82,Current!B$2:B$193,1,FALSE)</f>
         <v>textmsg_patch.php</v>
       </c>
     </row>
@@ -7541,10 +7648,10 @@
         <v>session_common.php</v>
       </c>
       <c r="F82" t="s">
-        <v>378</v>
+        <v>423</v>
       </c>
       <c r="G82" t="str">
-        <f>VLOOKUP(F82,Current!B$2:B$193,1,FALSE)</f>
+        <f>VLOOKUP(F83,Current!B$2:B$193,1,FALSE)</f>
         <v>textmsg_post.php</v>
       </c>
     </row>
@@ -7557,10 +7664,10 @@
         <v>session_delete.php</v>
       </c>
       <c r="F83" t="s">
-        <v>21</v>
+        <v>378</v>
       </c>
       <c r="G83" t="str">
-        <f>VLOOKUP(F83,Current!B$2:B$193,1,FALSE)</f>
+        <f>VLOOKUP(F84,Current!B$2:B$193,1,FALSE)</f>
         <v>visit.php</v>
       </c>
     </row>
@@ -7573,10 +7680,10 @@
         <v>session_get.php</v>
       </c>
       <c r="F84" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G84" t="str">
-        <f>VLOOKUP(F84,Current!B$2:B$193,1,FALSE)</f>
+        <f>VLOOKUP(F85,Current!B$2:B$193,1,FALSE)</f>
         <v>visit_common.php</v>
       </c>
     </row>
@@ -7589,10 +7696,10 @@
         <v>session_post.php</v>
       </c>
       <c r="F85" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G85" t="str">
-        <f>VLOOKUP(F85,Current!B$2:B$193,1,FALSE)</f>
+        <f>VLOOKUP(F86,Current!B$2:B$193,1,FALSE)</f>
         <v>visit_get.php</v>
       </c>
     </row>
@@ -7605,10 +7712,10 @@
         <v>staff.php</v>
       </c>
       <c r="F86" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G86" t="str">
-        <f>VLOOKUP(F86,Current!B$2:B$193,1,FALSE)</f>
+        <f>VLOOKUP(F87,Current!B$2:B$193,1,FALSE)</f>
         <v>visit_patch.php</v>
       </c>
     </row>
@@ -7621,10 +7728,10 @@
         <v>staffAddEdit.php</v>
       </c>
       <c r="F87" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G87" t="str">
-        <f>VLOOKUP(F87,Current!B$2:B$193,1,FALSE)</f>
+        <f>VLOOKUP(F88,Current!B$2:B$193,1,FALSE)</f>
         <v>visit_post.php</v>
       </c>
     </row>
@@ -7635,6 +7742,9 @@
       <c r="B88" t="str">
         <f>VLOOKUP(A88,Current!B$2:B$143,1,FALSE)</f>
         <v>staffAddEditText.php</v>
+      </c>
+      <c r="F88" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Tested for W3C errors: fixed all and updated docs.
</commit_message>
<xml_diff>
--- a/tools/web file descriptions.xlsx
+++ b/tools/web file descriptions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\bobw\Documents\GitHub\docsbydesign\piClinic\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{853EC751-0FF9-450E-8224-D566191458DB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0DA5055-CDF7-4C29-AFF2-198C6FE06408}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5934" yWindow="3396" windowWidth="20076" windowHeight="11286" tabRatio="388" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3036" yWindow="0" windowWidth="20076" windowHeight="11286" tabRatio="388" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Current" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1466" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1466" uniqueCount="452">
   <si>
     <t>addPatient.php</t>
   </si>
@@ -1270,9 +1270,6 @@
     <t>W3C OK</t>
   </si>
   <si>
-    <t>Error with &lt;style&gt; tags</t>
-  </si>
-  <si>
     <t>rptMonthlyPtSummHome.php</t>
   </si>
   <si>
@@ -1282,9 +1279,6 @@
     <t>adminHelpAddEdit.php</t>
   </si>
   <si>
-    <t>inDev</t>
-  </si>
-  <si>
     <t>Help text editing interface (dev)</t>
   </si>
   <si>
@@ -1424,6 +1418,18 @@
   </si>
   <si>
     <t>UI to print clinic visit form from</t>
+  </si>
+  <si>
+    <t>Not yet</t>
+  </si>
+  <si>
+    <t>Style tag errors</t>
+  </si>
+  <si>
+    <t>N/A (Redirect)</t>
+  </si>
+  <si>
+    <t>w3C OK</t>
   </si>
 </sst>
 </file>
@@ -1824,8 +1830,9 @@
   <dimension ref="A1:O158"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="618" topLeftCell="A73" activePane="bottomLeft"/>
-      <selection pane="bottomLeft" activeCell="F64" sqref="F64"/>
+      <pane ySplit="618" topLeftCell="A10"/>
+      <selection activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="D159" sqref="D159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2044,7 +2051,7 @@
         <v>352</v>
       </c>
       <c r="B7" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C7" t="s">
         <v>97</v>
@@ -2053,7 +2060,7 @@
         <v>240</v>
       </c>
       <c r="F7" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>221</v>
@@ -2061,36 +2068,26 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="4" t="s">
-        <v>352</v>
+        <v>384</v>
       </c>
       <c r="B8" t="s">
-        <v>401</v>
-      </c>
-      <c r="C8" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="C8" t="s">
         <v>31</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>240</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>403</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>405</v>
-      </c>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
+        <v>111</v>
+      </c>
+      <c r="G8" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="9" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="4" t="s">
@@ -2125,12 +2122,12 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="4" t="s">
-        <v>352</v>
+        <v>384</v>
       </c>
       <c r="B10" t="s">
-        <v>244</v>
-      </c>
-      <c r="C10" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="C10" t="s">
         <v>31</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -2140,22 +2137,11 @@
         <v>240</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1" t="str">
-        <f>VLOOKUP(B10,Profiled!A$1:A$98,1,FALSE)</f>
-        <v>adminHome.php</v>
-      </c>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
+        <v>348</v>
+      </c>
+      <c r="G10" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="4" t="s">
@@ -2203,10 +2189,10 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="4" t="s">
-        <v>352</v>
+        <v>384</v>
       </c>
       <c r="B13" t="s">
-        <v>272</v>
+        <v>409</v>
       </c>
       <c r="C13" t="s">
         <v>31</v>
@@ -2217,11 +2203,11 @@
       <c r="E13" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="F13" t="s">
-        <v>276</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>231</v>
+      <c r="F13" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="G13" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="14" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2255,10 +2241,10 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="4" t="s">
-        <v>352</v>
+        <v>384</v>
       </c>
       <c r="B15" t="s">
-        <v>281</v>
+        <v>399</v>
       </c>
       <c r="C15" t="s">
         <v>31</v>
@@ -2270,10 +2256,10 @@
         <v>240</v>
       </c>
       <c r="F15" t="s">
-        <v>292</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>231</v>
+        <v>343</v>
+      </c>
+      <c r="G15" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.55000000000000004">
@@ -2327,10 +2313,10 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="4" t="s">
-        <v>352</v>
+        <v>384</v>
       </c>
       <c r="B18" t="s">
-        <v>246</v>
+        <v>398</v>
       </c>
       <c r="C18" t="s">
         <v>31</v>
@@ -2338,18 +2324,20 @@
       <c r="D18" s="1" t="s">
         <v>397</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" t="s">
         <v>240</v>
       </c>
       <c r="F18" t="s">
-        <v>258</v>
+        <v>308</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="I18" s="1" t="str">
-        <f>VLOOKUP(B18,Profiled!A$1:A$98,1,FALSE)</f>
-        <v>adminShowUsers.php</v>
+        <v>220</v>
+      </c>
+      <c r="N18" t="s">
+        <v>313</v>
+      </c>
+      <c r="O18" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.55000000000000004">
@@ -2377,18 +2365,33 @@
         <v>352</v>
       </c>
       <c r="B20" t="s">
-        <v>353</v>
-      </c>
-      <c r="C20" t="s">
+        <v>400</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>222</v>
+        <v>448</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>401</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>222</v>
+        <v>402</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>403</v>
       </c>
       <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="4" t="s">
@@ -2479,7 +2482,7 @@
         <v>367</v>
       </c>
       <c r="B25" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C25" t="s">
         <v>29</v>
@@ -2488,7 +2491,7 @@
         <v>242</v>
       </c>
       <c r="F25" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.55000000000000004">
@@ -2564,51 +2567,39 @@
         <v>157</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="4" t="s">
         <v>352</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>65</v>
+      <c r="B29" t="s">
+        <v>244</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>240</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>60</v>
+        <v>257</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>217</v>
-      </c>
+        <v>221</v>
+      </c>
+      <c r="H29" s="1"/>
       <c r="I29" s="1" t="str">
         <f>VLOOKUP(B29,Profiled!A$1:A$98,1,FALSE)</f>
-        <v>clinicDash.php</v>
+        <v>adminHome.php</v>
       </c>
       <c r="J29" s="1"/>
-      <c r="K29" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="L29" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="M29" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="N29" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="O29" s="2" t="s">
-        <v>129</v>
-      </c>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="4" t="s">
@@ -2645,52 +2636,27 @@
         <v>157</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="4" t="s">
         <v>352</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="C31" s="1" t="s">
+      <c r="B31" t="s">
+        <v>272</v>
+      </c>
+      <c r="C31" t="s">
         <v>31</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>397</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>200</v>
+        <v>240</v>
+      </c>
+      <c r="F31" t="s">
+        <v>276</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="I31" s="1" t="e">
-        <f>VLOOKUP(B31,Profiled!A$1:A$98,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J31" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="K31" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="L31" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="M31" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="N31" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="O31" s="2" t="s">
-        <v>202</v>
+        <v>231</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.55000000000000004">
@@ -2969,20 +2935,23 @@
       <c r="A42" s="4" t="s">
         <v>352</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>382</v>
-      </c>
-      <c r="C42" s="1" t="s">
+      <c r="B42" t="s">
+        <v>281</v>
+      </c>
+      <c r="C42" t="s">
         <v>31</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>383</v>
+        <v>397</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="F42" t="s">
+        <v>292</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>222</v>
+        <v>231</v>
       </c>
     </row>
     <row r="43" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3357,7 +3326,7 @@
         <v>352</v>
       </c>
       <c r="B56" t="s">
-        <v>287</v>
+        <v>246</v>
       </c>
       <c r="C56" t="s">
         <v>31</v>
@@ -3369,10 +3338,14 @@
         <v>240</v>
       </c>
       <c r="F56" t="s">
-        <v>298</v>
+        <v>258</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>219</v>
+        <v>221</v>
+      </c>
+      <c r="I56" s="1" t="str">
+        <f>VLOOKUP(B56,Profiled!A$1:A$98,1,FALSE)</f>
+        <v>adminShowUsers.php</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.55000000000000004">
@@ -3380,7 +3353,7 @@
         <v>367</v>
       </c>
       <c r="B57" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C57" t="s">
         <v>29</v>
@@ -3389,7 +3362,7 @@
         <v>241</v>
       </c>
       <c r="F57" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="G57" s="1" t="s">
         <v>222</v>
@@ -3400,7 +3373,7 @@
         <v>367</v>
       </c>
       <c r="B58" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C58" t="s">
         <v>29</v>
@@ -3409,7 +3382,7 @@
         <v>242</v>
       </c>
       <c r="F58" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="G58" s="1" t="s">
         <v>222</v>
@@ -3429,7 +3402,7 @@
         <v>241</v>
       </c>
       <c r="F59" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="G59" s="1"/>
       <c r="I59" s="1"/>
@@ -3448,7 +3421,7 @@
         <v>242</v>
       </c>
       <c r="F60" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="G60" s="1"/>
       <c r="I60" s="1"/>
@@ -3467,7 +3440,7 @@
         <v>242</v>
       </c>
       <c r="F61" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="G61" s="1"/>
       <c r="I61" s="1"/>
@@ -3486,7 +3459,7 @@
         <v>242</v>
       </c>
       <c r="F62" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="G62" s="1"/>
       <c r="I62" s="1"/>
@@ -3506,7 +3479,7 @@
         <v>242</v>
       </c>
       <c r="F63" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="H63"/>
       <c r="I63"/>
@@ -3728,10 +3701,10 @@
         <v>352</v>
       </c>
       <c r="B71" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C71" t="s">
-        <v>31</v>
+        <v>223</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>222</v>
@@ -3742,7 +3715,6 @@
         <v>222</v>
       </c>
       <c r="H71"/>
-      <c r="I71"/>
       <c r="J71"/>
       <c r="K71"/>
       <c r="L71"/>
@@ -3781,20 +3753,20 @@
     </row>
     <row r="73" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="4" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B73" t="s">
+        <v>433</v>
+      </c>
+      <c r="C73" t="s">
         <v>435</v>
-      </c>
-      <c r="C73" t="s">
-        <v>437</v>
       </c>
       <c r="D73"/>
       <c r="E73" s="1" t="s">
         <v>239</v>
       </c>
       <c r="F73" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="G73" s="1" t="s">
         <v>222</v>
@@ -3810,20 +3782,20 @@
     </row>
     <row r="74" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="4" t="s">
+        <v>432</v>
+      </c>
+      <c r="B74" t="s">
         <v>434</v>
       </c>
-      <c r="B74" t="s">
-        <v>436</v>
-      </c>
       <c r="C74" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="D74"/>
       <c r="E74" s="1" t="s">
         <v>239</v>
       </c>
       <c r="F74" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="G74" s="1" t="s">
         <v>222</v>
@@ -3969,49 +3941,49 @@
         <v>157</v>
       </c>
     </row>
-    <row r="79" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:15" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="4" t="s">
         <v>352</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>397</v>
+        <v>449</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>240</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="H79" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="I79" s="1" t="e">
+      <c r="I79" s="1" t="str">
         <f>VLOOKUP(B79,Profiled!A$1:A$98,1,FALSE)</f>
-        <v>#N/A</v>
+        <v>clinicDash.php</v>
       </c>
       <c r="K79" s="1" t="s">
         <v>229</v>
       </c>
       <c r="L79" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="M79" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="N79" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="O79" s="1" t="s">
-        <v>131</v>
+        <v>229</v>
+      </c>
+      <c r="N79" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="O79" s="2" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="80" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4162,12 +4134,12 @@
         <v>157</v>
       </c>
     </row>
-    <row r="84" spans="1:15" s="1" customFormat="1" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:15" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="4" t="s">
         <v>352</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>89</v>
+        <v>189</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>31</v>
@@ -4176,34 +4148,38 @@
         <v>397</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>56</v>
+        <v>200</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="I84" s="1" t="s">
-        <v>271</v>
+        <v>222</v>
+      </c>
+      <c r="I84" s="1" t="e">
+        <f>VLOOKUP(B84,Profiled!A$1:A$98,1,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J84" s="1" t="s">
+        <v>222</v>
       </c>
       <c r="K84" s="1" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="L84" s="1" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="M84" s="1" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="N84" s="2" t="s">
-        <v>136</v>
+        <v>201</v>
       </c>
       <c r="O84" s="2" t="s">
-        <v>137</v>
+        <v>202</v>
       </c>
     </row>
     <row r="85" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4246,45 +4222,17 @@
         <v>352</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>90</v>
+        <v>382</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>397</v>
-      </c>
-      <c r="E86" s="1" t="s">
-        <v>240</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="D86" s="1"/>
       <c r="F86" s="1" t="s">
-        <v>55</v>
+        <v>383</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="H86" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="I86" s="1" t="e">
-        <f>VLOOKUP(B86,Profiled!A$1:A$98,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J86" s="1"/>
-      <c r="K86" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="L86" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="M86" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="N86" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="O86" s="1" t="s">
-        <v>139</v>
+        <v>222</v>
       </c>
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.55000000000000004">
@@ -4441,10 +4389,10 @@
       <c r="A91" s="4" t="s">
         <v>352</v>
       </c>
-      <c r="B91" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="C91" s="1" t="s">
+      <c r="B91" t="s">
+        <v>287</v>
+      </c>
+      <c r="C91" t="s">
         <v>31</v>
       </c>
       <c r="D91" s="1" t="s">
@@ -4453,34 +4401,11 @@
       <c r="E91" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="F91" s="1" t="s">
-        <v>116</v>
+      <c r="F91" t="s">
+        <v>298</v>
       </c>
       <c r="G91" s="1" t="s">
         <v>219</v>
-      </c>
-      <c r="H91" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="I91" s="1" t="e">
-        <f>VLOOKUP(B91,Profiled!A$1:A$98,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J91" s="1"/>
-      <c r="K91" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="L91" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="M91" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="N91" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="O91" s="1" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="92" spans="1:15" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -4534,7 +4459,7 @@
         <v>384</v>
       </c>
       <c r="B93" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C93" t="s">
         <v>223</v>
@@ -4546,7 +4471,7 @@
         <v>240</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="G93" t="s">
         <v>220</v>
@@ -4589,25 +4514,19 @@
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="4" t="s">
-        <v>384</v>
+        <v>352</v>
       </c>
       <c r="B95" t="s">
-        <v>406</v>
+        <v>354</v>
       </c>
       <c r="C95" t="s">
         <v>31</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>397</v>
-      </c>
-      <c r="E95" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="F95" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G95" t="s">
-        <v>220</v>
+        <v>450</v>
+      </c>
+      <c r="G95" s="1" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.55000000000000004">
@@ -4638,7 +4557,7 @@
         <v>384</v>
       </c>
       <c r="B97" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C97" t="s">
         <v>223</v>
@@ -4650,7 +4569,7 @@
         <v>240</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="G97" t="s">
         <v>220</v>
@@ -4681,7 +4600,7 @@
         <v>384</v>
       </c>
       <c r="B99" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C99" t="s">
         <v>97</v>
@@ -4693,7 +4612,7 @@
         <v>240</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="G99" t="s">
         <v>220</v>
@@ -4701,12 +4620,12 @@
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="4" t="s">
-        <v>384</v>
-      </c>
-      <c r="B100" t="s">
-        <v>408</v>
-      </c>
-      <c r="C100" t="s">
+        <v>352</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C100" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D100" s="1" t="s">
@@ -4716,10 +4635,33 @@
         <v>240</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>348</v>
-      </c>
-      <c r="G100" t="s">
-        <v>220</v>
+        <v>47</v>
+      </c>
+      <c r="G100" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="H100" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="I100" s="1" t="e">
+        <f>VLOOKUP(B100,Profiled!A$1:A$98,1,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J100" s="1"/>
+      <c r="K100" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="L100" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="M100" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="N100" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="O100" s="1" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="101" spans="1:15" x14ac:dyDescent="0.55000000000000004">
@@ -4750,7 +4692,7 @@
         <v>384</v>
       </c>
       <c r="B102" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C102" t="s">
         <v>223</v>
@@ -4762,20 +4704,20 @@
         <v>240</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="G102" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="1:15" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" s="4" t="s">
-        <v>384</v>
-      </c>
-      <c r="B103" t="s">
-        <v>411</v>
-      </c>
-      <c r="C103" t="s">
+        <v>352</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C103" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D103" s="1" t="s">
@@ -4785,10 +4727,32 @@
         <v>240</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="G103" t="s">
+        <v>56</v>
+      </c>
+      <c r="G103" s="1" t="s">
         <v>220</v>
+      </c>
+      <c r="H103" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="I103" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="J103" s="1"/>
+      <c r="K103" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="L103" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="M103" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="N103" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="O103" s="2" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="104" spans="1:15" x14ac:dyDescent="0.55000000000000004">
@@ -4796,7 +4760,7 @@
         <v>384</v>
       </c>
       <c r="B104" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C104" t="s">
         <v>223</v>
@@ -4808,7 +4772,7 @@
         <v>240</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="G104" t="s">
         <v>220</v>
@@ -4816,25 +4780,48 @@
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" s="4" t="s">
-        <v>384</v>
-      </c>
-      <c r="B105" t="s">
-        <v>400</v>
-      </c>
-      <c r="C105" t="s">
+        <v>352</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C105" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>222</v>
+        <v>397</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="F105" t="s">
-        <v>343</v>
-      </c>
-      <c r="G105" t="s">
-        <v>220</v>
+      <c r="F105" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G105" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="H105" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="I105" s="1" t="e">
+        <f>VLOOKUP(B105,Profiled!A$1:A$98,1,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J105" s="1"/>
+      <c r="K105" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="L105" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="M105" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="N105" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="O105" s="1" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="106" spans="1:15" x14ac:dyDescent="0.55000000000000004">
@@ -4842,7 +4829,7 @@
         <v>384</v>
       </c>
       <c r="B106" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C106" t="s">
         <v>223</v>
@@ -4854,7 +4841,7 @@
         <v>240</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="G106" t="s">
         <v>220</v>
@@ -5093,7 +5080,7 @@
         <v>367</v>
       </c>
       <c r="B114" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C114" t="s">
         <v>29</v>
@@ -5194,7 +5181,7 @@
         <v>367</v>
       </c>
       <c r="B118" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C118" t="s">
         <v>29</v>
@@ -5203,7 +5190,7 @@
         <v>242</v>
       </c>
       <c r="F118" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="G118" s="1" t="s">
         <v>221</v>
@@ -5283,31 +5270,48 @@
     </row>
     <row r="122" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" s="4" t="s">
-        <v>384</v>
-      </c>
-      <c r="B122" t="s">
-        <v>399</v>
-      </c>
-      <c r="C122" t="s">
+        <v>352</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="C122" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="E122" t="s">
+        <v>397</v>
+      </c>
+      <c r="E122" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="F122" t="s">
-        <v>308</v>
+      <c r="F122" s="1" t="s">
+        <v>116</v>
       </c>
       <c r="G122" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="N122" t="s">
-        <v>313</v>
-      </c>
-      <c r="O122" t="s">
-        <v>314</v>
+        <v>219</v>
+      </c>
+      <c r="H122" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="I122" s="1" t="e">
+        <f>VLOOKUP(B122,Profiled!A$1:A$98,1,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J122" s="1"/>
+      <c r="K122" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="L122" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="M122" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="N122" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="O122" s="1" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="123" spans="1:15" x14ac:dyDescent="0.55000000000000004">
@@ -5409,7 +5413,7 @@
     </row>
     <row r="127" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" s="4" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B127" t="s">
         <v>341</v>
@@ -5442,7 +5446,7 @@
         <v>241</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="G128" s="1"/>
       <c r="H128" s="1"/>
@@ -5469,7 +5473,7 @@
         <v>242</v>
       </c>
       <c r="F129" s="1" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="G129" s="1"/>
       <c r="H129" s="1"/>
@@ -5486,7 +5490,7 @@
         <v>367</v>
       </c>
       <c r="B130" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C130" t="s">
         <v>29</v>
@@ -5496,7 +5500,7 @@
         <v>242</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="G130" s="1"/>
       <c r="H130" s="1"/>
@@ -5523,7 +5527,7 @@
         <v>242</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="G131" s="1"/>
       <c r="H131" s="1"/>
@@ -5540,7 +5544,7 @@
         <v>367</v>
       </c>
       <c r="B132" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C132" t="s">
         <v>29</v>
@@ -5550,7 +5554,7 @@
         <v>242</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="G132" s="1"/>
       <c r="H132" s="1"/>
@@ -5577,7 +5581,7 @@
         <v>242</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="G133" s="1"/>
       <c r="H133" s="1"/>
@@ -5971,7 +5975,7 @@
         <v>31</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>397</v>
+        <v>451</v>
       </c>
       <c r="E147" s="1" t="s">
         <v>240</v>
@@ -6017,16 +6021,19 @@
         <v>352</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C149" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="D149" s="1" t="s">
+        <v>397</v>
+      </c>
       <c r="E149" s="1" t="s">
         <v>240</v>
       </c>
       <c r="F149" s="1" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="150" spans="1:15" x14ac:dyDescent="0.55000000000000004">
@@ -6342,7 +6349,7 @@
   </sheetData>
   <autoFilter ref="A1:O158" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:O158">
-      <sortCondition ref="B1:B158"/>
+      <sortCondition ref="A1:A158"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6373,14 +6380,14 @@
         <v>addComment.php</v>
       </c>
       <c r="F1" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="G1" t="str">
         <f>VLOOKUP(F1,Current!B$2:B$193,1,FALSE)</f>
         <v>adminBackup.php</v>
       </c>
       <c r="J1" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -6392,14 +6399,14 @@
         <v>addPatient.php</v>
       </c>
       <c r="F2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="G2" t="str">
         <f>VLOOKUP(F2,Current!B$2:B$193,1,FALSE)</f>
         <v>adminHelpAddEdit.php</v>
       </c>
       <c r="J2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -6908,7 +6915,7 @@
         <v>dbPass.php</v>
       </c>
       <c r="F30" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="G30" t="str">
         <f>VLOOKUP(F31,Current!B$2:B$193,1,FALSE)</f>
@@ -6924,7 +6931,7 @@
         <v>#N/A</v>
       </c>
       <c r="F31" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="G31" t="str">
         <f>VLOOKUP(F32,Current!B$2:B$193,1,FALSE)</f>
@@ -6940,7 +6947,7 @@
         <v>deletePatientImage.php</v>
       </c>
       <c r="F32" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="G32" t="str">
         <f>VLOOKUP(F33,Current!B$2:B$193,1,FALSE)</f>
@@ -6956,7 +6963,7 @@
         <v>endUiSession.php</v>
       </c>
       <c r="F33" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="G33" t="str">
         <f>VLOOKUP(F34,Current!B$2:B$193,1,FALSE)</f>
@@ -6972,7 +6979,7 @@
         <v>headTag.php</v>
       </c>
       <c r="F34" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="G34" t="str">
         <f>VLOOKUP(F35,Current!B$2:B$193,1,FALSE)</f>
@@ -6988,7 +6995,7 @@
         <v>helpHome.php</v>
       </c>
       <c r="F35" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="G35" t="str">
         <f>VLOOKUP(F36,Current!B$2:B$193,1,FALSE)</f>
@@ -7004,7 +7011,7 @@
         <v>helpHomeText.php</v>
       </c>
       <c r="F36" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="G36" t="str">
         <f>VLOOKUP(F37,Current!B$2:B$193,1,FALSE)</f>
@@ -7020,7 +7027,7 @@
         <v>icd.php</v>
       </c>
       <c r="F37" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="G37" t="str">
         <f>VLOOKUP(F38,Current!B$2:B$193,1,FALSE)</f>
@@ -7036,7 +7043,7 @@
         <v>icd_common.php</v>
       </c>
       <c r="F38" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="G38" t="str">
         <f>VLOOKUP(F39,Current!B$2:B$193,1,FALSE)</f>
@@ -7052,7 +7059,7 @@
         <v>icd_get.php</v>
       </c>
       <c r="F39" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="G39" t="str">
         <f>VLOOKUP(F40,Current!B$2:B$193,1,FALSE)</f>
@@ -7068,7 +7075,7 @@
         <v>icd_patch.php</v>
       </c>
       <c r="F40" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -7125,7 +7132,7 @@
         <v>image_get.php</v>
       </c>
       <c r="F44" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="G44" t="str">
         <f>VLOOKUP(F45,Current!B$2:B$193,1,FALSE)</f>
@@ -7285,7 +7292,7 @@
         <v>patient_post.php</v>
       </c>
       <c r="F54" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="G54" t="str">
         <f>VLOOKUP(F55,Current!B$2:B$193,1,FALSE)</f>
@@ -7301,7 +7308,7 @@
         <v>phpinfo.php</v>
       </c>
       <c r="F55" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="G55" t="str">
         <f>VLOOKUP(F56,Current!B$2:B$193,1,FALSE)</f>
@@ -7541,7 +7548,7 @@
         <v>rptDailyLogText.php</v>
       </c>
       <c r="F70" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="G70" t="str">
         <f>VLOOKUP(F71,Current!B$2:B$193,1,FALSE)</f>
@@ -7605,7 +7612,7 @@
         <v>#N/A</v>
       </c>
       <c r="F74" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="G74" t="str">
         <f>VLOOKUP(F75,Current!B$2:B$193,1,FALSE)</f>
@@ -7701,7 +7708,7 @@
         <v>securityText.php</v>
       </c>
       <c r="F80" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="G80" t="str">
         <f>VLOOKUP(F81,Current!B$2:B$193,1,FALSE)</f>
@@ -7733,7 +7740,7 @@
         <v>session_common.php</v>
       </c>
       <c r="F82" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="G82" t="str">
         <f>VLOOKUP(F83,Current!B$2:B$193,1,FALSE)</f>

</xml_diff>

<commit_message>
Updated with w3c validation error fixes
</commit_message>
<xml_diff>
--- a/tools/web file descriptions.xlsx
+++ b/tools/web file descriptions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\bobw\Documents\GitHub\docsbydesign\piClinic\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21DB6C95-A176-4F5B-BB3C-28F244436F18}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E27E0C83-8DAA-4831-9FBA-379CB4B8C732}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="816" yWindow="4386" windowWidth="22014" windowHeight="7680" tabRatio="388" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1454" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1488" uniqueCount="452">
   <si>
     <t>addPatient.php</t>
   </si>
@@ -1827,13 +1827,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
+  <sheetPr codeName="Sheet1" filterMode="1"/>
   <dimension ref="A1:P158"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="618" topLeftCell="A18" activePane="bottomLeft"/>
+      <pane ySplit="618" activePane="bottomLeft"/>
       <selection activeCell="D8" sqref="D8"/>
-      <selection pane="bottomLeft" activeCell="D29" sqref="D29:E29"/>
+      <selection pane="bottomLeft" activeCell="D135" sqref="D135:E158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2406,7 +2406,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:16" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="4" t="s">
         <v>379</v>
       </c>
@@ -2445,7 +2445,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:16" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="4" t="s">
         <v>379</v>
       </c>
@@ -2731,8 +2731,12 @@
       <c r="C31" t="s">
         <v>31</v>
       </c>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
+      <c r="D31" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>397</v>
+      </c>
       <c r="F31" s="1" t="s">
         <v>240</v>
       </c>
@@ -3419,8 +3423,12 @@
       <c r="C56" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
+      <c r="D56" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>397</v>
+      </c>
       <c r="F56" s="1" t="s">
         <v>240</v>
       </c>
@@ -4057,7 +4065,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="79" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:16" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="4" t="s">
         <v>379</v>
       </c>
@@ -4099,7 +4107,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="80" spans="1:16" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:16" s="1" customFormat="1" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="4" t="s">
         <v>379</v>
       </c>
@@ -4179,6 +4187,12 @@
       </c>
       <c r="C82" s="1" t="s">
         <v>31</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>397</v>
       </c>
       <c r="F82" s="1" t="s">
         <v>240</v>
@@ -4257,6 +4271,12 @@
       <c r="C84" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="D84" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>397</v>
+      </c>
       <c r="F84" s="1" t="s">
         <v>240</v>
       </c>
@@ -4373,7 +4393,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:16" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="4" t="s">
         <v>379</v>
       </c>
@@ -4418,7 +4438,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:16" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="4" t="s">
         <v>379</v>
       </c>
@@ -4507,8 +4527,12 @@
       <c r="C91" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D91" s="1"/>
-      <c r="E91" s="1"/>
+      <c r="D91" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>397</v>
+      </c>
       <c r="F91" s="1" t="s">
         <v>240</v>
       </c>
@@ -4542,7 +4566,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="92" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="4" t="s">
         <v>379</v>
       </c>
@@ -4657,8 +4681,12 @@
       <c r="C95" t="s">
         <v>31</v>
       </c>
-      <c r="D95" s="1"/>
-      <c r="E95" s="1"/>
+      <c r="D95" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>397</v>
+      </c>
       <c r="F95" s="1" t="s">
         <v>240</v>
       </c>
@@ -4669,7 +4697,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:16" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="4" t="s">
         <v>379</v>
       </c>
@@ -4769,8 +4797,12 @@
       <c r="C100" t="s">
         <v>31</v>
       </c>
-      <c r="D100" s="1"/>
-      <c r="E100" s="1"/>
+      <c r="D100" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>397</v>
+      </c>
       <c r="F100" s="1" t="s">
         <v>240</v>
       </c>
@@ -4781,7 +4813,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="1:16" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="4" t="s">
         <v>379</v>
       </c>
@@ -4837,8 +4869,12 @@
       <c r="C103" t="s">
         <v>31</v>
       </c>
-      <c r="D103" s="1"/>
-      <c r="E103" s="1"/>
+      <c r="D103" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>397</v>
+      </c>
       <c r="F103" s="1" t="s">
         <v>240</v>
       </c>
@@ -4883,8 +4919,12 @@
       <c r="C105" t="s">
         <v>31</v>
       </c>
-      <c r="D105" s="1"/>
-      <c r="E105" s="1"/>
+      <c r="D105" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>397</v>
+      </c>
       <c r="F105" s="1" t="s">
         <v>240</v>
       </c>
@@ -5357,8 +5397,12 @@
       <c r="C122" t="s">
         <v>31</v>
       </c>
-      <c r="D122" s="1"/>
-      <c r="E122" s="1"/>
+      <c r="D122" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>397</v>
+      </c>
       <c r="F122" t="s">
         <v>240</v>
       </c>
@@ -5697,8 +5741,12 @@
       <c r="C135" t="s">
         <v>31</v>
       </c>
-      <c r="D135" s="1"/>
-      <c r="E135" s="1"/>
+      <c r="D135" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="E135" s="1" t="s">
+        <v>397</v>
+      </c>
       <c r="F135" s="1" t="s">
         <v>240</v>
       </c>
@@ -6045,8 +6093,12 @@
       <c r="C147" t="s">
         <v>31</v>
       </c>
-      <c r="D147" s="1"/>
-      <c r="E147" s="1"/>
+      <c r="D147" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="E147" s="1" t="s">
+        <v>397</v>
+      </c>
       <c r="F147" s="1" t="s">
         <v>240</v>
       </c>
@@ -6096,8 +6148,12 @@
       <c r="C149" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D149" s="1"/>
-      <c r="E149" s="1"/>
+      <c r="D149" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="E149" s="1" t="s">
+        <v>397</v>
+      </c>
       <c r="F149" s="1" t="s">
         <v>240</v>
       </c>
@@ -6144,8 +6200,12 @@
       <c r="C151" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D151" s="1"/>
-      <c r="E151" s="1"/>
+      <c r="D151" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="E151" s="1" t="s">
+        <v>397</v>
+      </c>
       <c r="F151" s="1" t="s">
         <v>240</v>
       </c>
@@ -6218,8 +6278,12 @@
       <c r="C153" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D153" s="1"/>
-      <c r="E153" s="1"/>
+      <c r="D153" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="E153" s="1" t="s">
+        <v>397</v>
+      </c>
       <c r="F153" s="1" t="s">
         <v>240</v>
       </c>
@@ -6292,8 +6356,12 @@
       <c r="C155" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D155" s="1"/>
-      <c r="E155" s="1"/>
+      <c r="D155" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="E155" s="1" t="s">
+        <v>397</v>
+      </c>
       <c r="F155" s="1" t="s">
         <v>240</v>
       </c>
@@ -6377,8 +6445,12 @@
       <c r="C158" t="s">
         <v>31</v>
       </c>
-      <c r="D158" s="1"/>
-      <c r="E158" s="1"/>
+      <c r="D158" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="E158" s="1" t="s">
+        <v>397</v>
+      </c>
       <c r="F158" s="1" t="s">
         <v>240</v>
       </c>
@@ -6413,6 +6485,12 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:P158" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="reports"/>
+        <filter val="root"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="2">
       <filters>
         <filter val="UI"/>

</xml_diff>